<commit_message>
xlsx didnt save correctly? fixed
</commit_message>
<xml_diff>
--- a/[1]Atmega328p map & datasheet/Atmega328p.xlsx
+++ b/[1]Atmega328p map & datasheet/Atmega328p.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Interrupt" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Prescaler" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="WGM Interrupt Mode" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -622,7 +623,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">[3] WGM02
-Ser </t>
+Set </t>
         </r>
         <r>
           <rPr>
@@ -1945,8 +1946,1980 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Control Register B </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 109 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Force Output Compare A
+Only active when WGM Bits are non-PWM mode.
+[7] FOC0A 
+If Set, Compare Match is forced on Waveform Generation unit.
+This affects </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 6, PWM), based on </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">COM0A1:0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> in </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">TCCR0A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[6] FOC0B 
+If Set, Compare Match is forced on Waveform Generation unit.
+This affects </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 5, PWM), based on </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">COM0B1:0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> in </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">TCCR0A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[5] –	
+[4] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM01/00, found in TCCR0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[3] WGM02
+Set </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Prescaler, Timer/Counter0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[2] CS02
+[1] CS01 
+[0] CS00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter Control Register 2 B </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Datasheet page 158]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Force Output Compare A
+is only active when the WGM bits specify a non-PWM mode
+[7] FOC2A 
+If Set, Compare Match is forced on Waveform Generation unit.
+This affects </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC2A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 11, PWM), based on </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">COM2A1:0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> in </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">TCCR2A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[6] FOC2B 
+If Set, Compare Match is forced on Waveform Generation unit.
+This affects </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC2B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 3, PWM), based on </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">COM2A1:0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> in </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">TCCR2A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[5] -
+[4] -
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM21, WGM20, found in TCCR2A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[3] WGM22
+Set </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Prescaler, Timer/Counter2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[2] CS22
+[1] CS21
+[0] CS20</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Control Register B </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 109 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Force Output Compare A
+Only active when WGM Bits are non-PWM mode.
+[7] FOC0A 
+If Set, Compare Match is forced on Waveform Generation unit.
+This affects </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 6, PWM), based on </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">COM0A1:0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> in </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">TCCR0A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[6] FOC0B 
+If Set, Compare Match is forced on Waveform Generation unit.
+This affects </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 5, PWM), based on </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">COM0B1:0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> in </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">TCCR0A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[5] –	
+[4] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM01/00, found in TCCR0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[3] WGM02
+Set </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Prescaler, Timer/Counter0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[2] CS02
+[1] CS01 
+[0] CS00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter Control Register 2 B </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Datasheet page 158]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Force Output Compare A
+is only active when the WGM bits specify a non-PWM mode
+[7] FOC2A 
+If Set, Compare Match is forced on Waveform Generation unit.
+This affects </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC2A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 11, PWM), based on </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">COM2A1:0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> in </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">TCCR2A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[6] FOC2B 
+If Set, Compare Match is forced on Waveform Generation unit.
+This affects </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC2B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 3, PWM), based on </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">COM2A1:0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> in </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">TCCR2A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[5] -
+[4] -
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM21, WGM20, found in TCCR2A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[3] WGM22
+Set </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Prescaler, Timer/Counter2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[2] CS22
+[1] CS21
+[0] CS20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter1 Control Register B </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Datasheet page 136]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[7] ICNC1 : Input Capture Noise Canceler
+[6] ICES1	 : Input Capture Edge Select
+[5] -
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM11 and WGM10, found in TCCR1B, control the Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[4] WGM13 
+[3] WGM12 
+Set </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Preslacer, Timer/Counter1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[2] CS12 
+[1] CS11 
+[0] CS10</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 104 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output A Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 6, PWM) output behavior.
+[7] COM0A1 
+[6] COM0A0 
+Compare Match Output B Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 5, PWM) output behavior.
+[5] COM0B1 
+[4] COM0B0	
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM02, found in TCCR0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM01 
+[0] WGM00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter Control Register 2 A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Datasheet page 158]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output A Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC2A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 11, PWM) output behavior.
+[7] COM2A1 
+[6] COM2A0 
+Compare Match Output B Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC2B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 3, PWM) output behavior.
+[5] COM2B1 
+[4] COM2B0	
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM02, found in TCCR0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM21 
+[0] WGM20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter1 Control Register B </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Datasheet page 136]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[7] ICNC1 : Input Capture Noise Canceler
+[6] ICES1	 : Input Capture Edge Select
+[5] -
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM11 and WGM10, found in TCCR1B, control the Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[4] WGM13 
+[3] WGM12 
+Set </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Preslacer, Timer/Counter1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[2] CS12 
+[1] CS11 
+[0] CS10</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 104 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output A Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 6, PWM) output behavior.
+[7] COM0A1 
+[6] COM0A0 
+Compare Match Output B Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 5, PWM) output behavior.
+[5] COM0B1 
+[4] COM0B0	
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM02, found in TCCR0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM01 
+[0] WGM00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter Control Register 2 A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Datasheet page 158]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output A Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC2A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 11, PWM) output behavior.
+[7] COM2A1 
+[6] COM2A0 
+Compare Match Output B Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC2B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 3, PWM) output behavior.
+[5] COM2B1 
+[4] COM2B0	
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM02, found in TCCR0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM21 
+[0] WGM20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter1 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 135 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output Mode for Channel A
+[7] COM1A1 
+[6] COM1A0 
+Compare Match Output Mode for Channel B
+[5] COM0B1 
+[4] COM0B0	
+Controls the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 9, PWM) and </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 10, PWM) output behavior.
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM13 and WGM12, found in TCCR1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM11 
+[0] WGM10</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter1 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 135 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output Mode for Channel A
+[7] COM1A1 
+[6] COM1A0 
+Compare Match Output Mode for Channel B
+[5] COM0B1 
+[4] COM0B0	
+Controls the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 9, PWM) and </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 10, PWM) output behavior.
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM13 and WGM12, found in TCCR1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM11 
+[0] WGM10</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="299">
   <si>
     <t xml:space="preserve">Flash (Program FLash memory) [32K]</t>
   </si>
@@ -2657,6 +4630,192 @@
   </si>
   <si>
     <t xml:space="preserve">[x] Indicates bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCCR0B/1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2]CS02/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1]CS01/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0]CS00/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clock source (Timer/Counter stopped)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk I/O /(No prescaling)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk I/O 8 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk I/O 64 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk I/O 256 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk I/O 1024 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External clock source on T0/T1 pin. Clock on falling edge.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External clock source on T0/T1 pin. Clock on rising edge.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2]CS22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1]CS21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0]CS20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No clock source (Timer/Counter stopped).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk T2S (No prescaling)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk T2S 8 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk T2S 32 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk T2S 64 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk T2S 128 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk T 2 S 256 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk T 2 S 1024 (From prescaler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOV Flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM02/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM01/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM00/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCRx at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM, Phase Correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTTOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast PWM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xFFFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM, Ph Correct, 8-bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x00FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM, Ph Correct, 9-bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x01FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM, Ph Correct, 10-bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x03FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCR1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast PWM, 8-bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast PWM, 9-bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast PWM, 10-bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWM, Ph and Freq Correct </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Reserved)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast PWM</t>
   </si>
 </sst>
 </file>
@@ -2986,7 +5145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -3114,6 +5273,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -3191,7 +5371,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3434,6 +5614,30 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4231,8 +6435,8 @@
   </sheetPr>
   <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O30" activeCellId="0" sqref="O30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X26" activeCellId="0" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6494,17 +8698,492 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.48"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="61" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>246</v>
+      </c>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>248</v>
+      </c>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="61" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="62" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="62" t="s">
+        <v>253</v>
+      </c>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B17" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="62" t="s">
+        <v>255</v>
+      </c>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="62" t="s">
+        <v>256</v>
+      </c>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="62" t="s">
+        <v>257</v>
+      </c>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="62" t="s">
+        <v>258</v>
+      </c>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="62" t="s">
+        <v>259</v>
+      </c>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="D21:H21"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6512,5 +9191,815 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="6.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="61" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="61" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="61" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="61" width="9.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="61" width="8.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="61" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="F3" s="65" t="s">
+        <v>267</v>
+      </c>
+      <c r="G3" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="H3" s="66" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>271</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>274</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>271</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="H5" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="61" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>277</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="H6" s="61" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="61" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="F7" s="61" t="s">
+        <v>271</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="H7" s="61" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>274</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>277</v>
+      </c>
+      <c r="G9" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="H9" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>279</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>278</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>277</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="H11" s="61" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="I14" s="64" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="G15" s="65" t="s">
+        <v>267</v>
+      </c>
+      <c r="H15" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="I15" s="66" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="61" t="s">
+        <v>270</v>
+      </c>
+      <c r="G16" s="61" t="s">
+        <v>284</v>
+      </c>
+      <c r="H16" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="I16" s="61" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="61" t="s">
+        <v>285</v>
+      </c>
+      <c r="G17" s="61" t="s">
+        <v>286</v>
+      </c>
+      <c r="H17" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="I17" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="61" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="G18" s="61" t="s">
+        <v>288</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="I18" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="61" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="61" t="s">
+        <v>289</v>
+      </c>
+      <c r="G19" s="61" t="s">
+        <v>290</v>
+      </c>
+      <c r="H19" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="I19" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="61" t="n">
+        <v>4</v>
+      </c>
+      <c r="B20" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="G20" s="61" t="s">
+        <v>291</v>
+      </c>
+      <c r="H20" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="I20" s="61" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="B21" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="G21" s="61" t="s">
+        <v>286</v>
+      </c>
+      <c r="H21" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="I21" s="61" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="61" t="n">
+        <v>6</v>
+      </c>
+      <c r="B22" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="61" t="s">
+        <v>293</v>
+      </c>
+      <c r="G22" s="61" t="s">
+        <v>288</v>
+      </c>
+      <c r="H22" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="I22" s="61" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="61" t="n">
+        <v>7</v>
+      </c>
+      <c r="B23" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>294</v>
+      </c>
+      <c r="G23" s="61" t="s">
+        <v>290</v>
+      </c>
+      <c r="H23" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="I23" s="61" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="61" t="n">
+        <v>8</v>
+      </c>
+      <c r="B24" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="G24" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="H24" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="I24" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="61" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="61" t="s">
+        <v>295</v>
+      </c>
+      <c r="G25" s="61" t="s">
+        <v>291</v>
+      </c>
+      <c r="H25" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="I25" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="61" t="n">
+        <v>10</v>
+      </c>
+      <c r="B26" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="61" t="s">
+        <v>274</v>
+      </c>
+      <c r="G26" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="I26" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="61" t="n">
+        <v>11</v>
+      </c>
+      <c r="B27" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="61" t="s">
+        <v>274</v>
+      </c>
+      <c r="G27" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="H27" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="I27" s="61" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="61" t="n">
+        <v>12</v>
+      </c>
+      <c r="B28" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="61" t="s">
+        <v>276</v>
+      </c>
+      <c r="G28" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="H28" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="I28" s="61" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="61" t="n">
+        <v>13</v>
+      </c>
+      <c r="B29" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="61" t="s">
+        <v>297</v>
+      </c>
+      <c r="G29" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29" s="61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="61" t="n">
+        <v>14</v>
+      </c>
+      <c r="B30" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="G30" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="H30" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="I30" s="61" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="61" t="n">
+        <v>15</v>
+      </c>
+      <c r="B31" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="61" t="s">
+        <v>298</v>
+      </c>
+      <c r="G31" s="61" t="s">
+        <v>291</v>
+      </c>
+      <c r="H31" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="I31" s="61" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
downloaded newer datasheet, done first excersize
</commit_message>
<xml_diff>
--- a/[1]Atmega328p map & datasheet/Atmega328p.xlsx
+++ b/[1]Atmega328p map & datasheet/Atmega328p.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -82,7 +82,19 @@
 Timer Overflow flag
 TOV2  	Sets when TimerCounter2 overflows 
 	Executes TimerCounter2 Overflow Interrupt
-		TIMER2_OVF_vect</t>
+		TIMER2_OVF_vect
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Replies to the Question: Which OCRxX will be used?</t>
         </r>
       </text>
     </comment>
@@ -251,7 +263,19 @@
 Timer Overflow flag
 TOV1  	Sets when TimerCounter1 overflows 
 	Executes TimerCounter1 Overflow Interrupt
-		TIMER1_OVF_vect</t>
+		TIMER1_OVF_vect
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Replies to the Question: Which OCRxX will be used?</t>
         </r>
       </text>
     </comment>
@@ -373,6 +397,29 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">PORTB7 PORTB6 PORTB5 PORTB4 PORTB3 PORTB2 PORTB1 PORTB0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">First, set PORT input or output using DDRx
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 By setting a bit of PORT to 1:
 	if PORT is output, the output bit is set to HIGH.
 	if PORT is input, the internal pull-up resistor is activated
@@ -403,7 +450,19 @@
 Timer Overflow flag
 TOV0  	Sets when TimerCounter0 overflows 
 	Executes TimerCounter0 Overflow Interrupt
-		TIMER0_OVF_vect</t>
+		TIMER0_OVF_vect
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Replies to the Question: Which OCRxX will be used?</t>
         </r>
       </text>
     </comment>
@@ -927,6 +986,28 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">PORTD6 PORTD5 PORTD4 PORTD3 PORTD2 PORTD1 PORTD0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">First, set PORT input or output using DDRx
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 By setting a bit of PORT to 1:
 	if PORT is output, the output bit is set to HIGH.
 	if PORT is input, the internal pull-up resistor is activated
@@ -1567,6 +1648,28 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">	-	PORTC6 PORTC5 PORTC4 PORTC3 PORTC2 PORTC1 PORTC0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">First, set PORT input or output using DDRx
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 By setting a bit of PORT to 1:
 	if PORT is output, the output bit is set to HIGH.
 	if PORT is input, the internal pull-up resistor is activated
@@ -4752,7 +4855,7 @@
     <t xml:space="preserve">CTC</t>
   </si>
   <si>
-    <t xml:space="preserve">OCRA</t>
+    <t xml:space="preserve">OCRxX</t>
   </si>
   <si>
     <t xml:space="preserve">Fast PWM </t>
@@ -4825,7 +4928,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4998,6 +5101,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -5009,7 +5120,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -5371,7 +5481,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5620,7 +5730,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5637,6 +5747,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5740,7 +5854,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>386280</xdr:colOff>
+      <xdr:colOff>385560</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
@@ -5751,8 +5865,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18437400" y="254160"/>
-          <a:ext cx="1862280" cy="1179000"/>
+          <a:off x="18438120" y="254160"/>
+          <a:ext cx="1860840" cy="1179000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5833,9 +5947,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>142200</xdr:colOff>
+      <xdr:colOff>141480</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5844,8 +5958,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17727120" y="1233360"/>
-          <a:ext cx="340200" cy="1379880"/>
+          <a:off x="17727480" y="1233360"/>
+          <a:ext cx="339840" cy="1379160"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5911,7 +6025,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>438120</xdr:colOff>
+      <xdr:colOff>437400</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
@@ -5922,8 +6036,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18341640" y="1893960"/>
-          <a:ext cx="1394640" cy="336600"/>
+          <a:off x="18342360" y="1893960"/>
+          <a:ext cx="1393200" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5988,9 +6102,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>141120</xdr:colOff>
+      <xdr:colOff>140400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5999,8 +6113,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17726040" y="2622240"/>
-          <a:ext cx="340200" cy="3483720"/>
+          <a:off x="17726400" y="2622240"/>
+          <a:ext cx="339840" cy="3483000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6066,7 +6180,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>336240</xdr:colOff>
+      <xdr:colOff>335520</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
@@ -6077,8 +6191,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18181080" y="4222800"/>
-          <a:ext cx="1453320" cy="336600"/>
+          <a:off x="18181800" y="4222800"/>
+          <a:ext cx="1451880" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6143,9 +6257,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>120600</xdr:colOff>
+      <xdr:colOff>119880</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
+      <xdr:rowOff>34920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6154,8 +6268,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17705520" y="6127920"/>
-          <a:ext cx="340200" cy="2172600"/>
+          <a:off x="17705880" y="6127920"/>
+          <a:ext cx="339840" cy="2171880"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6221,7 +6335,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>79560</xdr:colOff>
+      <xdr:colOff>78840</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
@@ -6233,7 +6347,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="19367280" y="7232040"/>
-          <a:ext cx="2471760" cy="336600"/>
+          <a:ext cx="2471040" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6282,9 +6396,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>613080</xdr:colOff>
+      <xdr:colOff>612360</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6297,8 +6411,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11235240" y="6224400"/>
-          <a:ext cx="5391000" cy="1119600"/>
+          <a:off x="11235960" y="6224400"/>
+          <a:ext cx="5390280" cy="1118880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6319,9 +6433,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6335,7 +6449,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="20449440" y="1835280"/>
-          <a:ext cx="4577760" cy="3029400"/>
+          <a:ext cx="4578840" cy="3028680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6356,9 +6470,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>135360</xdr:colOff>
+      <xdr:colOff>134640</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>172440</xdr:rowOff>
+      <xdr:rowOff>171720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6367,8 +6481,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17720280" y="517320"/>
-          <a:ext cx="340200" cy="706680"/>
+          <a:off x="17720640" y="517320"/>
+          <a:ext cx="339840" cy="705960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6435,11 +6549,11 @@
   </sheetPr>
   <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X26" activeCellId="0" sqref="X26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X15" activeCellId="0" sqref="X15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="8.72"/>
@@ -6450,7 +6564,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="8.72"/>
@@ -6460,7 +6574,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="9.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="29" style="1" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="8.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8700,16 +8813,14 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9202,17 +9313,17 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="6.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="61" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="61" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="61" width="17.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="61" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="61" width="9.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="61" width="9.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="61" width="8.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="61" width="11.52"/>
   </cols>
@@ -9339,7 +9450,7 @@
       <c r="E6" s="61" t="s">
         <v>276</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="67" t="s">
         <v>277</v>
       </c>
       <c r="G6" s="61" t="s">
@@ -9417,7 +9528,7 @@
       <c r="E9" s="61" t="s">
         <v>274</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="67" t="s">
         <v>277</v>
       </c>
       <c r="G9" s="61" t="s">
@@ -9469,7 +9580,7 @@
       <c r="E11" s="61" t="s">
         <v>278</v>
       </c>
-      <c r="F11" s="61" t="s">
+      <c r="F11" s="67" t="s">
         <v>277</v>
       </c>
       <c r="G11" s="61" t="s">

</xml_diff>

<commit_message>
done excersize 2, fixed an old example
</commit_message>
<xml_diff>
--- a/[1]Atmega328p map & datasheet/Atmega328p.xlsx
+++ b/[1]Atmega328p map & datasheet/Atmega328p.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -253,6 +253,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">IF ANY Of THE BITS ARE SET, ISR(...VECT){} MUST BE INCLUDED</t>
         </r>
@@ -1969,6 +1970,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">IF ANY Of THE BITS ARE SET, ISR(...VECT){} MUST BE INCLUDED</t>
         </r>
@@ -3634,6 +3636,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="E6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Carefull: if you need to use both OCR0A and OCR0B, once one of them matches the timer, the timer0 will reset.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E14" authorId="0">
       <text>
         <r>
@@ -5033,7 +5049,7 @@
     <t xml:space="preserve">CTC</t>
   </si>
   <si>
-    <t xml:space="preserve">OCRxX</t>
+    <t xml:space="preserve">OCR0A and OCR0B</t>
   </si>
   <si>
     <t xml:space="preserve">Fast PWM </t>
@@ -5353,7 +5369,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5532,13 +5548,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -6171,7 +6180,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6183,10 +6192,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6196,6 +6201,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6299,7 +6308,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>384840</xdr:colOff>
+      <xdr:colOff>384480</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
@@ -6311,7 +6320,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18438120" y="254160"/>
-          <a:ext cx="1860120" cy="1179000"/>
+          <a:ext cx="1859760" cy="1179000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6392,9 +6401,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>140760</xdr:colOff>
+      <xdr:colOff>140400</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6404,7 +6413,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17727480" y="1233360"/>
-          <a:ext cx="339120" cy="1378440"/>
+          <a:ext cx="338760" cy="1378080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6470,7 +6479,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>436680</xdr:colOff>
+      <xdr:colOff>436320</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
@@ -6482,7 +6491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18342360" y="1893960"/>
-          <a:ext cx="1392480" cy="336600"/>
+          <a:ext cx="1392120" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6547,9 +6556,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>139680</xdr:colOff>
+      <xdr:colOff>139320</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6559,7 +6568,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17726400" y="2622240"/>
-          <a:ext cx="339120" cy="3482280"/>
+          <a:ext cx="338760" cy="3481920"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6625,7 +6634,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>334800</xdr:colOff>
+      <xdr:colOff>334440</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
@@ -6637,7 +6646,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18181800" y="4222800"/>
-          <a:ext cx="1451160" cy="336600"/>
+          <a:ext cx="1450800" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6702,9 +6711,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>119160</xdr:colOff>
+      <xdr:colOff>118800</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>34200</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6714,7 +6723,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17705880" y="6127920"/>
-          <a:ext cx="339120" cy="2171160"/>
+          <a:ext cx="338760" cy="2170800"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6780,7 +6789,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>78120</xdr:colOff>
+      <xdr:colOff>77760</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
@@ -6792,7 +6801,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="19367280" y="7232040"/>
-          <a:ext cx="2470320" cy="336600"/>
+          <a:ext cx="2469960" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6841,9 +6850,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>611640</xdr:colOff>
+      <xdr:colOff>611280</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6857,7 +6866,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11235960" y="6224400"/>
-          <a:ext cx="5389560" cy="1118160"/>
+          <a:ext cx="5389200" cy="1117800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6878,9 +6887,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>240840</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:rowOff>131040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6894,7 +6903,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="20449440" y="1835280"/>
-          <a:ext cx="4583880" cy="3027960"/>
+          <a:ext cx="4585320" cy="3027600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6915,9 +6924,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>133920</xdr:colOff>
+      <xdr:colOff>133560</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6927,7 +6936,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17720640" y="517320"/>
-          <a:ext cx="339120" cy="705240"/>
+          <a:ext cx="338760" cy="704880"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6994,11 +7003,11 @@
   </sheetPr>
   <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y26" activeCellId="0" sqref="Y26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R11" activeCellId="0" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="8.72"/>
@@ -9258,8 +9267,8 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10071,7 +10080,7 @@
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
@@ -10529,16 +10538,16 @@
       <c r="J21" s="68"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="60" t="s">
         <v>301</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10569,7 +10578,7 @@
     <mergeCell ref="A23:H23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A23" r:id="rId2" display="https://eleccelerator.com/avr-timer-calculator/"/>
+    <hyperlink ref="A23" r:id="rId2" display="Prescaler Calculator: https://eleccelerator.com/avr-timer-calculator/ "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -10593,305 +10602,305 @@
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="69" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="70" t="s">
         <v>303</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="70" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="72" t="n">
+      <c r="A2" s="71" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="72" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="72" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="72" t="n">
+      <c r="A3" s="71" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="72" t="s">
         <v>307</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="72" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="72" t="n">
+      <c r="A4" s="71" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="72" t="s">
         <v>309</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="72" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="72" t="n">
+      <c r="A5" s="71" t="n">
         <v>6</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="72" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="72" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="72" t="n">
+      <c r="A6" s="71" t="n">
         <v>8</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="72" t="s">
         <v>313</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="72" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="72" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="72" t="s">
         <v>315</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="72" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="72" t="s">
         <v>318</v>
       </c>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="72" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="72" t="s">
         <v>320</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="72" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="72" t="n">
+      <c r="A10" s="71" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="72" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="72" t="n">
+      <c r="A11" s="71" t="n">
         <v>12</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="72" t="s">
         <v>322</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="72" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="72" t="n">
+      <c r="A12" s="71" t="n">
         <v>14</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="72" t="s">
         <v>324</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="72" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="72" t="n">
+      <c r="A13" s="71" t="n">
         <v>16</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="72" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="72" t="n">
+      <c r="A14" s="71" t="n">
         <v>18</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="72" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="72" t="s">
         <v>328</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="72" t="s">
         <v>329</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="72" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="72" t="s">
         <v>331</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="72" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="72" t="s">
         <v>333</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="72" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="72" t="n">
+      <c r="A18" s="71" t="n">
         <v>20</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="72" t="s">
         <v>335</v>
       </c>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="72" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="72" t="n">
+      <c r="A19" s="71" t="n">
         <v>22</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="72" t="s">
         <v>337</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="72" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="72" t="n">
+      <c r="A20" s="71" t="n">
         <v>24</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="72" t="s">
         <v>339</v>
       </c>
-      <c r="C20" s="66" t="s">
+      <c r="C20" s="72" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="72" t="n">
+      <c r="A21" s="71" t="n">
         <v>26</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="72" t="s">
         <v>341</v>
       </c>
-      <c r="C21" s="66" t="s">
+      <c r="C21" s="72" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="72" t="n">
+      <c r="A22" s="71" t="n">
         <v>28</v>
       </c>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="72" t="s">
         <v>343</v>
       </c>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="72" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="72" t="s">
         <v>345</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="72" t="s">
         <v>346</v>
       </c>
-      <c r="C23" s="66" t="s">
+      <c r="C23" s="72" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="72" t="s">
         <v>348</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="72" t="s">
         <v>349</v>
       </c>
-      <c r="C24" s="66" t="s">
+      <c r="C24" s="72" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="72" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="72" t="s">
         <v>352</v>
       </c>
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="72" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="72" t="n">
+      <c r="A26" s="71" t="n">
         <v>30</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="72" t="s">
         <v>354</v>
       </c>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="72" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="72" t="n">
+      <c r="A27" s="71" t="n">
         <v>32</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="72" t="s">
         <v>356</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="72" t="s">
         <v>357</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dont know what changed
</commit_message>
<xml_diff>
--- a/[1]Atmega328p map & datasheet/Atmega328p.xlsx
+++ b/[1]Atmega328p map & datasheet/Atmega328p.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="WGM Interrupt Mode" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Prescaler" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Int Vectors" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="External Interrupt" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -293,20 +294,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="R45" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">X-, Y- and Z-pointer registers can be set to index any register in the file</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="S7" authorId="0">
       <text>
         <r>
@@ -635,6 +622,67 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Replies to the Question: Which OCRxX will be used?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">–	–	–	–	–	–	INT1 INT0
+External Interrupt Mask Register
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] INT1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> External Interrupt Request 1 Enable
+	When the INT1 bit is set, the external pin interrupt is enabled.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[0] INT0:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> External Interrupt Request 0 Enable
+	When the INT0 bit is set, the external pin interrupt is enabled.</t>
         </r>
       </text>
     </comment>
@@ -1444,6 +1492,119 @@
         </r>
       </text>
     </comment>
+    <comment ref="X17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">–	–	–	–	ISC11 ISC10 ISC01 ISC00
+External Interrupt Control Register A
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[3] ISC11:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Interrupt Sense Control 1 Bit 1 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[2] ISC10: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Interrupt Sense Control 1 Bit 0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] ISC01: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Interrupt Sense Control 0 Bit 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[0] ISC00: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Interrupt Sense Control 0 Bit 0</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="X19" authorId="0">
       <text>
         <r>
@@ -4285,7 +4446,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="367">
   <si>
     <t xml:space="preserve">Flash (Program FLash memory) [32K]</t>
   </si>
@@ -4983,21 +5144,6 @@
     <t xml:space="preserve">F8H</t>
   </si>
   <si>
-    <t xml:space="preserve">Extended I/O space, only the ST/STS/STD and LD/LDS/LDD instructions can be used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X-Register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y-Register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-Register</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[x] Indicates bit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Update of</t>
   </si>
   <si>
@@ -5359,6 +5505,48 @@
   </si>
   <si>
     <t xml:space="preserve">Store Program Memory Read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISC11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISC10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT1 External Interrupt Request 1 [PD3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The low level of INT1 generates an interrupt request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any logical change on INT1 generates an interrupt request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The falling edge of INT1 generates an interrupt request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The rising edge of INT1 generates an interrupt request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISC01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISC00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Interrupt Request 0 [PD2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The low level of INT0 generates an interrupt request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any logical change on INT0 generates an interrupt request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The falling edge of INT0 generates an interrupt request.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The rising edge of INT0 generates an interrupt request.</t>
   </si>
 </sst>
 </file>
@@ -5369,7 +5557,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5556,12 +5744,25 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5636,6 +5837,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF314004"/>
+        <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF3465A4"/>
         <bgColor rgb="FF2A6099"/>
       </patternFill>
@@ -5644,12 +5851,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFCC0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF472702"/>
-        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
     <fill>
@@ -5667,7 +5868,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF158466"/>
-        <bgColor rgb="FF008080"/>
+        <bgColor rgb="FF2A6099"/>
       </patternFill>
     </fill>
     <fill>
@@ -5686,6 +5887,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2A6099"/>
         <bgColor rgb="FF3465A4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0084D1"/>
+        <bgColor rgb="FF0563C1"/>
       </patternFill>
     </fill>
   </fills>
@@ -6056,15 +6263,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="13" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="13" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="14" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="15" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6076,7 +6287,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="15" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6136,30 +6347,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6176,7 +6363,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6192,6 +6379,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6205,6 +6396,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6266,7 +6473,7 @@
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FFBF0041"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0084D1"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -6287,7 +6494,7 @@
       <rgbColor rgb="FF404040"/>
       <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF472702"/>
+      <rgbColor rgb="FF314004"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF55308D"/>
@@ -6704,182 +6911,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>461520</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>118800</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17705880" y="6127920"/>
-          <a:ext cx="338760" cy="2170800"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="955" h="6045">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:cubicBezTo>
-                <a:pt x="238" y="0"/>
-                <a:pt x="477" y="251"/>
-                <a:pt x="477" y="503"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="477" y="2518"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="477" y="2770"/>
-                <a:pt x="715" y="3022"/>
-                <a:pt x="954" y="3022"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="715" y="3022"/>
-                <a:pt x="477" y="3273"/>
-                <a:pt x="477" y="3525"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="477" y="5540"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="477" y="5792"/>
-                <a:pt x="238" y="6044"/>
-                <a:pt x="0" y="6044"/>
-              </a:cubicBezTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>69120</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>77760</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>4680</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19367280" y="7232040"/>
-          <a:ext cx="2469960" cy="336600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>and the next 2048 locations address the internal data SRAM.</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>183240</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>611280</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11235960" y="6224400"/>
-          <a:ext cx="5389200" cy="1117800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>536040</xdr:colOff>
       <xdr:row>10</xdr:row>
@@ -6893,11 +6924,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 2" descr=""/>
+        <xdr:cNvPr id="5" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -6930,7 +6961,7 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7001,10 +7032,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AO53"/>
+  <dimension ref="A1:AO54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R11" activeCellId="0" sqref="R11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA17" activeCellId="0" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7653,7 +7684,7 @@
       <c r="S11" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="T11" s="24" t="s">
+      <c r="T11" s="35" t="s">
         <v>105</v>
       </c>
       <c r="U11" s="24" t="s">
@@ -7668,7 +7699,7 @@
       <c r="X11" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="Y11" s="35" t="s">
+      <c r="Y11" s="36" t="s">
         <v>80</v>
       </c>
       <c r="Z11" s="33" t="s">
@@ -7712,16 +7743,16 @@
       <c r="Q12" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="R12" s="36" t="s">
+      <c r="R12" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="S12" s="37" t="s">
+      <c r="S12" s="38" t="s">
         <v>111</v>
       </c>
       <c r="T12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="U12" s="38" t="s">
+      <c r="U12" s="39" t="s">
         <v>112</v>
       </c>
       <c r="V12" s="28" t="s">
@@ -7747,7 +7778,7 @@
       <c r="AF12" s="8"/>
       <c r="AG12" s="8"/>
       <c r="AH12" s="8"/>
-      <c r="AI12" s="39"/>
+      <c r="AI12" s="40"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
@@ -7790,7 +7821,7 @@
       <c r="X13" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="Y13" s="36" t="s">
+      <c r="Y13" s="37" t="s">
         <v>101</v>
       </c>
       <c r="Z13" s="33" t="s">
@@ -7804,7 +7835,7 @@
       <c r="AF13" s="8"/>
       <c r="AG13" s="8"/>
       <c r="AH13" s="8"/>
-      <c r="AI13" s="39"/>
+      <c r="AI13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
@@ -7899,7 +7930,7 @@
       <c r="Q15" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="R15" s="40" t="s">
+      <c r="R15" s="41" t="s">
         <v>137</v>
       </c>
       <c r="S15" s="28" t="s">
@@ -7952,13 +7983,13 @@
       <c r="M16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="N16" s="38" t="s">
+      <c r="N16" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="O16" s="38" t="s">
+      <c r="O16" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="P16" s="38" t="s">
+      <c r="P16" s="39" t="s">
         <v>112</v>
       </c>
       <c r="Q16" s="11" t="s">
@@ -7982,10 +8013,10 @@
       <c r="W16" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="X16" s="41" t="s">
+      <c r="X16" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="Y16" s="41" t="s">
+      <c r="Y16" s="42" t="s">
         <v>147</v>
       </c>
       <c r="Z16" s="33" t="s">
@@ -7999,7 +8030,7 @@
       <c r="AF16" s="8"/>
       <c r="AG16" s="8"/>
       <c r="AH16" s="8"/>
-      <c r="AI16" s="39"/>
+      <c r="AI16" s="40"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
@@ -8021,10 +8052,10 @@
       <c r="Q17" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="R17" s="42" t="s">
+      <c r="R17" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="S17" s="42" t="s">
+      <c r="S17" s="43" t="s">
         <v>151</v>
       </c>
       <c r="T17" s="28" t="s">
@@ -8039,10 +8070,10 @@
       <c r="W17" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="X17" s="41" t="s">
+      <c r="X17" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="Y17" s="41" t="s">
+      <c r="Y17" s="42" t="s">
         <v>156</v>
       </c>
       <c r="Z17" s="33" t="s">
@@ -8056,7 +8087,7 @@
       <c r="AF17" s="8"/>
       <c r="AG17" s="8"/>
       <c r="AH17" s="8"/>
-      <c r="AI17" s="39"/>
+      <c r="AI17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
@@ -8099,7 +8130,7 @@
       <c r="X18" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="Y18" s="42" t="s">
+      <c r="Y18" s="43" t="s">
         <v>159</v>
       </c>
       <c r="Z18" s="33" t="s">
@@ -8113,7 +8144,7 @@
       <c r="AF18" s="8"/>
       <c r="AG18" s="8"/>
       <c r="AH18" s="8"/>
-      <c r="AI18" s="39"/>
+      <c r="AI18" s="40"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
@@ -8141,28 +8172,28 @@
       <c r="Q19" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="R19" s="43" t="s">
+      <c r="R19" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="S19" s="44" t="s">
+      <c r="S19" s="45" t="s">
         <v>163</v>
       </c>
       <c r="T19" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="U19" s="45" t="s">
+      <c r="U19" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="V19" s="44" t="s">
+      <c r="V19" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="W19" s="45" t="s">
+      <c r="W19" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="X19" s="45" t="s">
+      <c r="X19" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="Y19" s="46" t="s">
+      <c r="Y19" s="47" t="s">
         <v>168</v>
       </c>
       <c r="Z19" s="33" t="s">
@@ -8176,7 +8207,7 @@
       <c r="AF19" s="8"/>
       <c r="AG19" s="8"/>
       <c r="AH19" s="8"/>
-      <c r="AI19" s="39"/>
+      <c r="AI19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
@@ -8210,10 +8241,10 @@
       <c r="S20" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="T20" s="47" t="s">
+      <c r="T20" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="U20" s="47" t="s">
+      <c r="U20" s="48" t="s">
         <v>174</v>
       </c>
       <c r="V20" s="28" t="s">
@@ -8225,7 +8256,7 @@
       <c r="X20" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="Y20" s="38" t="s">
+      <c r="Y20" s="39" t="s">
         <v>142</v>
       </c>
       <c r="Z20" s="33" t="s">
@@ -8239,7 +8270,7 @@
       <c r="AF20" s="8"/>
       <c r="AG20" s="8"/>
       <c r="AH20" s="8"/>
-      <c r="AI20" s="39"/>
+      <c r="AI20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
@@ -8279,16 +8310,16 @@
       <c r="U21" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="V21" s="48" t="s">
+      <c r="V21" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="W21" s="48" t="s">
+      <c r="W21" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="X21" s="49" t="s">
+      <c r="X21" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="Y21" s="49" t="s">
+      <c r="Y21" s="50" t="s">
         <v>181</v>
       </c>
       <c r="Z21" s="33" t="s">
@@ -8302,7 +8333,7 @@
       <c r="AF21" s="8"/>
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
-      <c r="AI21" s="39"/>
+      <c r="AI21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
@@ -8322,19 +8353,19 @@
       <c r="M22" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="N22" s="42" t="s">
+      <c r="N22" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="O22" s="42" t="s">
+      <c r="O22" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="P22" s="42" t="s">
+      <c r="P22" s="43" t="s">
         <v>151</v>
       </c>
       <c r="Q22" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="R22" s="50" t="s">
+      <c r="R22" s="51" t="s">
         <v>80</v>
       </c>
       <c r="S22" s="28" t="s">
@@ -8369,7 +8400,7 @@
       <c r="AF22" s="8"/>
       <c r="AG22" s="8"/>
       <c r="AH22" s="8"/>
-      <c r="AI22" s="39"/>
+      <c r="AI22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
@@ -8426,7 +8457,7 @@
       <c r="AF23" s="8"/>
       <c r="AG23" s="8"/>
       <c r="AH23" s="8"/>
-      <c r="AI23" s="39"/>
+      <c r="AI23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
@@ -8485,7 +8516,7 @@
       <c r="AF24" s="8"/>
       <c r="AG24" s="8"/>
       <c r="AH24" s="8"/>
-      <c r="AI24" s="39"/>
+      <c r="AI24" s="40"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
@@ -8542,7 +8573,7 @@
       <c r="AF25" s="8"/>
       <c r="AG25" s="8"/>
       <c r="AH25" s="8"/>
-      <c r="AI25" s="39"/>
+      <c r="AI25" s="40"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
@@ -8573,19 +8604,19 @@
       <c r="T26" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="U26" s="36" t="s">
+      <c r="U26" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="V26" s="36" t="s">
+      <c r="V26" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="W26" s="37" t="s">
+      <c r="W26" s="38" t="s">
         <v>198</v>
       </c>
       <c r="X26" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="Y26" s="38" t="s">
+      <c r="Y26" s="39" t="s">
         <v>141</v>
       </c>
       <c r="Z26" s="33" t="s">
@@ -8599,7 +8630,7 @@
       <c r="AF26" s="8"/>
       <c r="AG26" s="8"/>
       <c r="AH26" s="8"/>
-      <c r="AI26" s="39"/>
+      <c r="AI26" s="40"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
@@ -8642,7 +8673,7 @@
       <c r="X27" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="Y27" s="35" t="s">
+      <c r="Y27" s="36" t="s">
         <v>206</v>
       </c>
       <c r="Z27" s="33" t="s">
@@ -8656,7 +8687,7 @@
       <c r="AF27" s="8"/>
       <c r="AG27" s="8"/>
       <c r="AH27" s="8"/>
-      <c r="AI27" s="39"/>
+      <c r="AI27" s="40"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
@@ -8699,7 +8730,7 @@
       <c r="X28" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="Y28" s="35" t="s">
+      <c r="Y28" s="36" t="s">
         <v>214</v>
       </c>
       <c r="Z28" s="33" t="s">
@@ -8713,7 +8744,7 @@
       <c r="AF28" s="8"/>
       <c r="AG28" s="8"/>
       <c r="AH28" s="8"/>
-      <c r="AI28" s="39"/>
+      <c r="AI28" s="40"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
@@ -8770,7 +8801,7 @@
       <c r="AF29" s="8"/>
       <c r="AG29" s="8"/>
       <c r="AH29" s="8"/>
-      <c r="AI29" s="39"/>
+      <c r="AI29" s="40"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
@@ -8829,7 +8860,7 @@
       <c r="AF30" s="8"/>
       <c r="AG30" s="8"/>
       <c r="AH30" s="8"/>
-      <c r="AI30" s="39"/>
+      <c r="AI30" s="40"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
@@ -8886,7 +8917,7 @@
       <c r="AF31" s="8"/>
       <c r="AG31" s="8"/>
       <c r="AH31" s="8"/>
-      <c r="AI31" s="39"/>
+      <c r="AI31" s="40"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
@@ -8943,7 +8974,7 @@
       <c r="AF32" s="8"/>
       <c r="AG32" s="8"/>
       <c r="AH32" s="8"/>
-      <c r="AI32" s="39"/>
+      <c r="AI32" s="40"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
@@ -9000,7 +9031,7 @@
       <c r="AF33" s="8"/>
       <c r="AG33" s="8"/>
       <c r="AH33" s="8"/>
-      <c r="AI33" s="39"/>
+      <c r="AI33" s="40"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
@@ -9057,7 +9088,7 @@
       <c r="AF34" s="8"/>
       <c r="AG34" s="8"/>
       <c r="AH34" s="8"/>
-      <c r="AI34" s="39"/>
+      <c r="AI34" s="40"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
@@ -9097,10 +9128,10 @@
       <c r="W35" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="X35" s="51" t="s">
+      <c r="X35" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="Y35" s="52" t="s">
+      <c r="Y35" s="53" t="s">
         <v>230</v>
       </c>
       <c r="Z35" s="33" t="s">
@@ -9114,139 +9145,114 @@
       <c r="AF35" s="8"/>
       <c r="AG35" s="8"/>
       <c r="AH35" s="8"/>
-      <c r="AI35" s="39"/>
+      <c r="AI35" s="40"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P36" s="1"/>
-      <c r="Q36" s="53"/>
-      <c r="Z36" s="54"/>
+      <c r="Q36" s="54"/>
+      <c r="Z36" s="55"/>
       <c r="AA36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P37" s="1"/>
-      <c r="Q37" s="53"/>
-      <c r="Z37" s="54"/>
+      <c r="Q37" s="54"/>
+      <c r="Z37" s="55"/>
       <c r="AA37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P38" s="1"/>
-      <c r="Q38" s="53"/>
-      <c r="Z38" s="54"/>
+      <c r="Q38" s="54"/>
+      <c r="Z38" s="55"/>
       <c r="AA38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P39" s="1"/>
-      <c r="Q39" s="53"/>
-      <c r="Z39" s="54"/>
+      <c r="Q39" s="54"/>
+      <c r="Z39" s="55"/>
       <c r="AA39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P40" s="1"/>
-      <c r="Q40" s="53"/>
-      <c r="Z40" s="54"/>
+      <c r="Q40" s="54"/>
+      <c r="Z40" s="55"/>
       <c r="AA40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P41" s="1"/>
-      <c r="Q41" s="53"/>
-      <c r="Z41" s="54"/>
+      <c r="Q41" s="54"/>
+      <c r="Z41" s="55"/>
       <c r="AA41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P42" s="1"/>
-      <c r="Q42" s="53"/>
-      <c r="Z42" s="54"/>
+      <c r="Q42" s="1"/>
+      <c r="Z42" s="55"/>
       <c r="AA42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P43" s="1"/>
-      <c r="Q43" s="53"/>
-      <c r="Z43" s="54"/>
+      <c r="Q43" s="1"/>
+      <c r="Z43" s="55"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P44" s="1"/>
-      <c r="Q44" s="53"/>
-      <c r="R44" s="55"/>
-      <c r="S44" s="56" t="s">
-        <v>232</v>
-      </c>
-      <c r="T44" s="56"/>
-      <c r="U44" s="56"/>
-      <c r="V44" s="56"/>
-      <c r="W44" s="56"/>
-      <c r="X44" s="56"/>
-      <c r="Y44" s="56"/>
-      <c r="Z44" s="56"/>
+      <c r="Q44" s="1"/>
+      <c r="Z44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P45" s="1"/>
-      <c r="Q45" s="53"/>
-      <c r="R45" s="57"/>
-      <c r="S45" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="Z45" s="54"/>
+      <c r="Q45" s="1"/>
+      <c r="Z45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P46" s="1"/>
-      <c r="Q46" s="53"/>
-      <c r="R46" s="58"/>
-      <c r="S46" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="Z46" s="54"/>
+      <c r="Q46" s="1"/>
+      <c r="Z46" s="55"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P47" s="1"/>
-      <c r="Q47" s="53"/>
-      <c r="R47" s="59"/>
-      <c r="S47" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z47" s="54"/>
+      <c r="Q47" s="1"/>
+      <c r="Z47" s="55"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P48" s="1"/>
-      <c r="Q48" s="53"/>
-      <c r="Z48" s="54"/>
+      <c r="Q48" s="1"/>
+      <c r="Z48" s="55"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P49" s="1"/>
-      <c r="Q49" s="53"/>
-      <c r="Z49" s="54"/>
+      <c r="Q49" s="1"/>
+      <c r="Z49" s="55"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P50" s="1"/>
-      <c r="Q50" s="53"/>
-      <c r="Z50" s="54"/>
+      <c r="Q50" s="1"/>
+      <c r="Z50" s="55"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P51" s="1"/>
-      <c r="Q51" s="53"/>
-      <c r="R51" s="60" t="s">
-        <v>236</v>
-      </c>
-      <c r="S51" s="60"/>
-      <c r="Z51" s="54"/>
+      <c r="Q51" s="1"/>
+      <c r="Z51" s="55"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P52" s="1"/>
-      <c r="Q52" s="53"/>
-      <c r="Z52" s="54"/>
+      <c r="Q52" s="1"/>
+      <c r="Z52" s="55"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P53" s="1"/>
-      <c r="Q53" s="53"/>
-      <c r="Z53" s="54"/>
+      <c r="Q53" s="1"/>
+      <c r="Z53" s="55"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q54" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="I1:P1"/>
     <mergeCell ref="Q1:Z1"/>
     <mergeCell ref="AA1:AI1"/>
-    <mergeCell ref="S44:Z44"/>
-    <mergeCell ref="R51:S51"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -9267,29 +9273,29 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="6.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="61" width="10.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="61" width="17.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="61" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="61" width="9.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="61" width="8.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="61" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="56" width="6.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="56" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="56" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="56" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="56" width="9.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="56" width="8.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="56" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="39" t="s">
         <v>112</v>
       </c>
     </row>
@@ -9297,251 +9303,251 @@
       <c r="B2" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>237</v>
       </c>
-      <c r="H2" s="62" t="s">
+      <c r="E3" s="58" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="63" t="s">
+      <c r="F3" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="G3" s="59" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="H3" s="59" t="s">
         <v>241</v>
       </c>
-      <c r="D3" s="38" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="56" t="s">
         <v>242</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="F4" s="56" t="s">
         <v>243</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="G4" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="G3" s="64" t="s">
+      <c r="H4" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="H3" s="64" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="56" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="61" t="n">
+      <c r="F5" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="61" t="n">
+      <c r="C6" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="61" t="n">
+      <c r="E6" s="56" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="56" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="61" t="n">
+      <c r="C7" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>250</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="56" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="D8" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="56" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="G9" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="H9" s="56" t="s">
         <v>247</v>
       </c>
-      <c r="F4" s="61" t="s">
-        <v>248</v>
-      </c>
-      <c r="G4" s="61" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="56" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>250</v>
+      </c>
+      <c r="F11" s="60" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="61" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="61" t="s">
-        <v>251</v>
-      </c>
-      <c r="F5" s="61" t="s">
-        <v>248</v>
-      </c>
-      <c r="G5" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="H5" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="61" t="s">
-        <v>253</v>
-      </c>
-      <c r="F6" s="65" t="s">
-        <v>254</v>
-      </c>
-      <c r="G6" s="61" t="s">
-        <v>249</v>
-      </c>
-      <c r="H6" s="61" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="61" t="s">
-        <v>255</v>
-      </c>
-      <c r="F7" s="61" t="s">
-        <v>248</v>
-      </c>
-      <c r="G7" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="H7" s="61" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="61" t="s">
-        <v>256</v>
-      </c>
-      <c r="F8" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="61" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="61" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>251</v>
-      </c>
-      <c r="F9" s="65" t="s">
-        <v>254</v>
-      </c>
-      <c r="G9" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="H9" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="61" t="s">
-        <v>256</v>
-      </c>
-      <c r="F10" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="61" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="61" t="s">
-        <v>255</v>
-      </c>
-      <c r="F11" s="65" t="s">
-        <v>254</v>
-      </c>
-      <c r="G11" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="H11" s="61" t="s">
-        <v>244</v>
+      <c r="G11" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="H11" s="56" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9551,510 +9557,510 @@
       <c r="C14" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="62" t="s">
-        <v>237</v>
-      </c>
-      <c r="I14" s="62" t="s">
+      <c r="H14" s="57" t="s">
+        <v>232</v>
+      </c>
+      <c r="I14" s="57" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="F15" s="58" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="63" t="s">
+      <c r="G15" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="H15" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="I15" s="59" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="G16" s="56" t="s">
+        <v>256</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="I16" s="56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="56" t="s">
         <v>257</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="G17" s="56" t="s">
         <v>258</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="H17" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="I17" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="56" t="s">
         <v>259</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="G18" s="56" t="s">
         <v>260</v>
       </c>
-      <c r="F15" s="63" t="s">
-        <v>243</v>
-      </c>
-      <c r="G15" s="63" t="s">
+      <c r="H18" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="I18" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="56" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="G19" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="H19" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="I19" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="56" t="n">
+        <v>4</v>
+      </c>
+      <c r="B20" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>248</v>
+      </c>
+      <c r="G20" s="56" t="s">
+        <v>263</v>
+      </c>
+      <c r="H20" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="H15" s="64" t="s">
+      <c r="I20" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="I15" s="64" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="56" t="n">
+        <v>5</v>
+      </c>
+      <c r="B21" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="56" t="s">
+        <v>264</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>258</v>
+      </c>
+      <c r="H21" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I21" s="56" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="56" t="n">
+        <v>6</v>
+      </c>
+      <c r="B22" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="56" t="s">
+        <v>265</v>
+      </c>
+      <c r="G22" s="56" t="s">
+        <v>260</v>
+      </c>
+      <c r="H22" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I22" s="56" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="56" t="n">
+        <v>7</v>
+      </c>
+      <c r="B23" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="56" t="s">
+        <v>266</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="H23" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I23" s="56" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="56" t="n">
+        <v>8</v>
+      </c>
+      <c r="B24" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="56" t="s">
+        <v>267</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>268</v>
+      </c>
+      <c r="H24" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I24" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="56" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="56" t="s">
+        <v>267</v>
+      </c>
+      <c r="G25" s="56" t="s">
+        <v>263</v>
+      </c>
+      <c r="H25" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I25" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="56" t="n">
+        <v>10</v>
+      </c>
+      <c r="B26" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="56" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="61" t="n">
+      <c r="G26" s="56" t="s">
+        <v>268</v>
+      </c>
+      <c r="H26" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="I26" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="56" t="n">
+        <v>11</v>
+      </c>
+      <c r="B27" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="B16" s="61" t="n">
+      <c r="D27" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G27" s="56" t="s">
+        <v>268</v>
+      </c>
+      <c r="H27" s="56" t="s">
+        <v>239</v>
+      </c>
+      <c r="I27" s="56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="56" t="n">
+        <v>12</v>
+      </c>
+      <c r="B28" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="C16" s="61" t="n">
+      <c r="E28" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="61" t="n">
+      <c r="F28" s="56" t="s">
+        <v>248</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>268</v>
+      </c>
+      <c r="H28" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="I28" s="56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="56" t="n">
+        <v>13</v>
+      </c>
+      <c r="B29" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="E16" s="61" t="n">
+      <c r="E29" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="56" t="s">
+        <v>269</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29" s="56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="56" t="n">
+        <v>14</v>
+      </c>
+      <c r="B30" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="61" t="s">
+      <c r="F30" s="56" t="s">
+        <v>270</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>268</v>
+      </c>
+      <c r="H30" s="56" t="s">
         <v>247</v>
       </c>
-      <c r="G16" s="61" t="s">
-        <v>261</v>
-      </c>
-      <c r="H16" s="61" t="s">
-        <v>249</v>
-      </c>
-      <c r="I16" s="61" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="61" t="n">
+      <c r="I30" s="56" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="56" t="n">
+        <v>15</v>
+      </c>
+      <c r="B31" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="61" t="n">
+      <c r="C31" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="61" t="s">
-        <v>262</v>
-      </c>
-      <c r="G17" s="61" t="s">
+      <c r="D31" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" s="56" t="s">
+        <v>270</v>
+      </c>
+      <c r="G31" s="56" t="s">
         <v>263</v>
       </c>
-      <c r="H17" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="I17" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="61" t="n">
-        <v>2</v>
-      </c>
-      <c r="B18" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="61" t="s">
-        <v>264</v>
-      </c>
-      <c r="G18" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="H18" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="I18" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="61" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="61" t="s">
-        <v>266</v>
-      </c>
-      <c r="G19" s="61" t="s">
-        <v>267</v>
-      </c>
-      <c r="H19" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="I19" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="61" t="n">
-        <v>4</v>
-      </c>
-      <c r="B20" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="61" t="s">
-        <v>253</v>
-      </c>
-      <c r="G20" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="H20" s="61" t="s">
-        <v>249</v>
-      </c>
-      <c r="I20" s="61" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="61" t="n">
-        <v>5</v>
-      </c>
-      <c r="B21" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="61" t="s">
-        <v>269</v>
-      </c>
-      <c r="G21" s="61" t="s">
-        <v>263</v>
-      </c>
-      <c r="H21" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="I21" s="61" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="61" t="n">
-        <v>6</v>
-      </c>
-      <c r="B22" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="61" t="s">
-        <v>270</v>
-      </c>
-      <c r="G22" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="H22" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="I22" s="61" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="61" t="n">
-        <v>7</v>
-      </c>
-      <c r="B23" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="61" t="s">
-        <v>271</v>
-      </c>
-      <c r="G23" s="61" t="s">
-        <v>267</v>
-      </c>
-      <c r="H23" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="I23" s="61" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="61" t="n">
-        <v>8</v>
-      </c>
-      <c r="B24" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="61" t="s">
-        <v>272</v>
-      </c>
-      <c r="G24" s="61" t="s">
-        <v>273</v>
-      </c>
-      <c r="H24" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="I24" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="61" t="n">
-        <v>9</v>
-      </c>
-      <c r="B25" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" s="61" t="s">
-        <v>272</v>
-      </c>
-      <c r="G25" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="H25" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="I25" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="61" t="n">
-        <v>10</v>
-      </c>
-      <c r="B26" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="61" t="s">
-        <v>251</v>
-      </c>
-      <c r="G26" s="61" t="s">
-        <v>273</v>
-      </c>
-      <c r="H26" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="I26" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="61" t="n">
-        <v>11</v>
-      </c>
-      <c r="B27" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="F27" s="61" t="s">
-        <v>251</v>
-      </c>
-      <c r="G27" s="61" t="s">
-        <v>273</v>
-      </c>
-      <c r="H27" s="61" t="s">
-        <v>244</v>
-      </c>
-      <c r="I27" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="61" t="n">
-        <v>12</v>
-      </c>
-      <c r="B28" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="61" t="s">
-        <v>253</v>
-      </c>
-      <c r="G28" s="61" t="s">
-        <v>273</v>
-      </c>
-      <c r="H28" s="61" t="s">
-        <v>249</v>
-      </c>
-      <c r="I28" s="61" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="61" t="n">
-        <v>13</v>
-      </c>
-      <c r="B29" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="F29" s="61" t="s">
-        <v>274</v>
-      </c>
-      <c r="G29" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="I29" s="61" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="61" t="n">
-        <v>14</v>
-      </c>
-      <c r="B30" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D30" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="61" t="s">
-        <v>275</v>
-      </c>
-      <c r="G30" s="61" t="s">
-        <v>273</v>
-      </c>
-      <c r="H30" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="I30" s="61" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="61" t="n">
-        <v>15</v>
-      </c>
-      <c r="B31" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D31" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="F31" s="61" t="s">
-        <v>275</v>
-      </c>
-      <c r="G31" s="61" t="s">
-        <v>268</v>
-      </c>
-      <c r="H31" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="I31" s="61" t="s">
-        <v>244</v>
+      <c r="H31" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I31" s="56" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -10076,8 +10082,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10088,7 +10094,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>52</v>
@@ -10108,219 +10114,219 @@
       <c r="G1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>276</v>
+      </c>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="62" t="s">
         <v>277</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="62" t="s">
         <v>278</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="62" t="s">
         <v>279</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="62" t="s">
         <v>280</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="n">
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="B3" s="61" t="n">
+      <c r="C8" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>281</v>
+      </c>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="67" t="s">
-        <v>281</v>
-      </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="61" t="n">
+      <c r="D9" s="62" t="s">
+        <v>282</v>
+      </c>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="67" t="s">
-        <v>282</v>
-      </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" s="61" t="n">
+      <c r="B10" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="67" t="s">
+      <c r="C10" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="62" t="s">
         <v>283</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="67" t="s">
-        <v>284</v>
-      </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>285</v>
-      </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="67" t="s">
-        <v>286</v>
-      </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="67" t="s">
-        <v>287</v>
-      </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="68"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="67" t="s">
-        <v>288</v>
-      </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
@@ -10334,220 +10340,220 @@
       <c r="G12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="56" t="s">
+        <v>284</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>285</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>286</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="62" t="s">
+        <v>288</v>
+      </c>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="62" t="s">
         <v>289</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="62" t="s">
         <v>290</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B17" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="D13" s="66" t="s">
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="62" t="s">
         <v>292</v>
       </c>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="61"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="61" t="n">
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="B14" s="61" t="n">
+      <c r="C19" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="62" t="s">
+        <v>293</v>
+      </c>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="67" t="s">
-        <v>293</v>
-      </c>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="B15" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="61" t="n">
+      <c r="D20" s="62" t="s">
+        <v>294</v>
+      </c>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="67" t="s">
-        <v>294</v>
-      </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="68"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="B16" s="61" t="n">
+      <c r="B21" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="67" t="s">
+      <c r="C21" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="B17" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D17" s="67" t="s">
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="64" t="s">
         <v>296</v>
       </c>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="68"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B18" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="67" t="s">
-        <v>297</v>
-      </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B19" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" s="67" t="s">
-        <v>298</v>
-      </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="68"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="67" t="s">
-        <v>299</v>
-      </c>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="68"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="B21" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="61" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="67" t="s">
-        <v>300</v>
-      </c>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="60" t="s">
-        <v>301</v>
-      </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10598,8 +10604,8 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10608,300 +10614,300 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="65" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>298</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>300</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="67" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="68" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="C3" s="68" t="s">
         <v>303</v>
       </c>
-      <c r="C1" s="70" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="67" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="68" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="72" t="s">
+      <c r="C4" s="68" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="72" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="67" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" s="68" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="71" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="72" t="s">
+      <c r="C5" s="68" t="s">
         <v>307</v>
       </c>
-      <c r="C3" s="72" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="67" t="n">
+        <v>8</v>
+      </c>
+      <c r="B6" s="68" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="71" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="72" t="s">
+      <c r="C6" s="68" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="68" t="s">
         <v>309</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="B7" s="68" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="71" t="n">
-        <v>6</v>
-      </c>
-      <c r="B5" s="72" t="s">
+      <c r="C7" s="68" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="72" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="68" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="71" t="n">
-        <v>8</v>
-      </c>
-      <c r="B6" s="72" t="s">
+      <c r="B8" s="68" t="s">
         <v>313</v>
       </c>
-      <c r="C6" s="72" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="72" t="s">
+      <c r="C8" s="68" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="72" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="68" t="s">
         <v>315</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="B9" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="68" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="72" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="67" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="67" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" s="68" t="s">
         <v>317</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="C11" s="68" t="s">
         <v>318</v>
       </c>
-      <c r="C8" s="72" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="67" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" s="68" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="72" t="s">
+      <c r="C12" s="68" t="s">
         <v>320</v>
       </c>
-      <c r="B9" s="72" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="67" t="n">
+        <v>16</v>
+      </c>
+      <c r="B13" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="67" t="n">
+        <v>18</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="68" t="s">
+        <v>323</v>
+      </c>
+      <c r="B15" s="68" t="s">
+        <v>324</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="68" t="s">
+        <v>326</v>
+      </c>
+      <c r="B16" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="68" t="s">
+        <v>328</v>
+      </c>
+      <c r="B17" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="67" t="n">
+        <v>20</v>
+      </c>
+      <c r="B18" s="68" t="s">
+        <v>330</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="67" t="n">
         <v>22</v>
       </c>
-      <c r="C9" s="72" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="71" t="n">
-        <v>10</v>
-      </c>
-      <c r="B10" s="72" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="72" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="71" t="n">
-        <v>12</v>
-      </c>
-      <c r="B11" s="72" t="s">
-        <v>322</v>
-      </c>
-      <c r="C11" s="72" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="71" t="n">
-        <v>14</v>
-      </c>
-      <c r="B12" s="72" t="s">
-        <v>324</v>
-      </c>
-      <c r="C12" s="72" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="71" t="n">
-        <v>16</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="72" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="71" t="n">
-        <v>18</v>
-      </c>
-      <c r="B14" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="72" t="s">
-        <v>328</v>
-      </c>
-      <c r="B15" s="72" t="s">
-        <v>329</v>
-      </c>
-      <c r="C15" s="72" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="72" t="s">
-        <v>331</v>
-      </c>
-      <c r="B16" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="72" t="s">
+      <c r="B19" s="68" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="72" t="s">
+      <c r="C19" s="68" t="s">
         <v>333</v>
       </c>
-      <c r="B17" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="72" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="67" t="n">
+        <v>24</v>
+      </c>
+      <c r="B20" s="68" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="71" t="n">
-        <v>20</v>
-      </c>
-      <c r="B18" s="72" t="s">
+      <c r="C20" s="68" t="s">
         <v>335</v>
       </c>
-      <c r="C18" s="72" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="67" t="n">
+        <v>26</v>
+      </c>
+      <c r="B21" s="68" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="71" t="n">
-        <v>22</v>
-      </c>
-      <c r="B19" s="72" t="s">
+      <c r="C21" s="68" t="s">
         <v>337</v>
       </c>
-      <c r="C19" s="72" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="67" t="n">
+        <v>28</v>
+      </c>
+      <c r="B22" s="68" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="71" t="n">
-        <v>24</v>
-      </c>
-      <c r="B20" s="72" t="s">
+      <c r="C22" s="68" t="s">
         <v>339</v>
       </c>
-      <c r="C20" s="72" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="68" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="71" t="n">
-        <v>26</v>
-      </c>
-      <c r="B21" s="72" t="s">
+      <c r="B23" s="68" t="s">
         <v>341</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C23" s="68" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="71" t="n">
-        <v>28</v>
-      </c>
-      <c r="B22" s="72" t="s">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="68" t="s">
         <v>343</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="B24" s="68" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="72" t="s">
+      <c r="C24" s="68" t="s">
         <v>345</v>
       </c>
-      <c r="B23" s="72" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="68" t="s">
         <v>346</v>
       </c>
-      <c r="C23" s="72" t="s">
+      <c r="B25" s="68" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="72" t="s">
+      <c r="C25" s="68" t="s">
         <v>348</v>
       </c>
-      <c r="B24" s="72" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="67" t="n">
+        <v>30</v>
+      </c>
+      <c r="B26" s="68" t="s">
         <v>349</v>
       </c>
-      <c r="C24" s="72" t="s">
+      <c r="C26" s="68" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="72" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="67" t="n">
+        <v>32</v>
+      </c>
+      <c r="B27" s="68" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="C27" s="68" t="s">
         <v>352</v>
-      </c>
-      <c r="C25" s="72" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="71" t="n">
-        <v>30</v>
-      </c>
-      <c r="B26" s="72" t="s">
-        <v>354</v>
-      </c>
-      <c r="C26" s="72" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="71" t="n">
-        <v>32</v>
-      </c>
-      <c r="B27" s="72" t="s">
-        <v>356</v>
-      </c>
-      <c r="C27" s="72" t="s">
-        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -10913,4 +10919,245 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="56" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="70" t="s">
+        <v>353</v>
+      </c>
+      <c r="B3" s="70" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>355</v>
+      </c>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>357</v>
+      </c>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>358</v>
+      </c>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="70" t="s">
+        <v>360</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>361</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>362</v>
+      </c>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>363</v>
+      </c>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="71" t="s">
+        <v>364</v>
+      </c>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>365</v>
+      </c>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed excersizes, added excel code
</commit_message>
<xml_diff>
--- a/[1]Atmega328p map & datasheet/Atmega328p.xlsx
+++ b/[1]Atmega328p map & datasheet/Atmega328p.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,8 @@
     <sheet name="Prescaler" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Int Vectors" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="External Interrupt" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="PWM COMxx AnalogWrite" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Logic Gates" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -659,7 +661,29 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> External Interrupt Request 1 Enable
-	When the INT1 bit is set, the external pin interrupt is enabled.
+	When the INT1 bit is set, the external pin interrupt is enabled. </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[PD3]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -682,7 +706,18 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve"> External Interrupt Request 0 Enable
-	When the INT0 bit is set, the external pin interrupt is enabled.</t>
+	When the INT0 bit is set, the external pin interrupt is enabled. </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[PD2]</t>
         </r>
       </text>
     </comment>
@@ -1526,16 +1561,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Interrupt Sense Control 1 Bit 1 
+          <t xml:space="preserve"> Interrupt Sense Control 1 Bit 1 
 </t>
         </r>
         <r>
@@ -2195,8 +2221,8 @@
 [7] COM1A1 
 [6] COM1A0 
 Compare Match Output Mode for Channel B
-[5] COM0B1 
-[4] COM0B0	
+[5] COM1B1 
+[4] COM1B0	
 Controls the </t>
         </r>
         <r>
@@ -4445,8 +4471,819 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 104 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output A Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 6, PWM) output behavior.
+[7] COM0A1 
+[6] COM0A0 
+Compare Match Output B Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 5, PWM) output behavior.
+[5] COM0B1 
+[4] COM0B0	
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM02, found in TCCR0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM01 
+[0] WGM00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 104 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output A Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 6, PWM) output behavior.
+[7] COM0A1 
+[6] COM0A0 
+Compare Match Output B Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 5, PWM) output behavior.
+[5] COM0B1 
+[4] COM0B0	
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM02, found in TCCR0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM01 
+[0] WGM00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 104 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output A Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 6, PWM) output behavior.
+[7] COM0A1 
+[6] COM0A0 
+Compare Match Output B Mode
+Control the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 5, PWM) output behavior.
+[5] COM0B1 
+[4] COM0B0	
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM02, found in TCCR0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM01 
+[0] WGM00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter1 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 135 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output Mode for Channel A
+[7] COM1A1 
+[6] COM1A0 
+Compare Match Output Mode for Channel B
+[5] COM1B1 
+[4] COM1B0	
+Controls the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 9, PWM) and </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 10, PWM) output behavior.
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM13 and WGM12, found in TCCR1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM11 
+[0] WGM10</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter1 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 135 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output Mode for Channel A
+[7] COM1A1 
+[6] COM1A0 
+Compare Match Output Mode for Channel B
+[5] COM1B1 
+[4] COM1B0	
+Controls the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 9, PWM) and </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 10, PWM) output behavior.
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM13 and WGM12, found in TCCR1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM11 
+[0] WGM10</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter1 Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[Page 135 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output Mode for Channel A
+[7] COM1A1 
+[6] COM1A0 
+Compare Match Output Mode for Channel B
+[5] COM1B1 
+[4] COM1B0	
+Controls the </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 9, PWM) and </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">OC1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> (Pin 10, PWM) output behavior.
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM13 and WGM12, found in TCCR1B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM11 
+[0] WGM10</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="400">
   <si>
     <t xml:space="preserve">Flash (Program FLash memory) [32K]</t>
   </si>
@@ -4925,6 +5762,9 @@
     <t xml:space="preserve">77H</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">TIMSK2</t>
   </si>
   <si>
@@ -5018,6 +5858,12 @@
     <t xml:space="preserve">3FFF</t>
   </si>
   <si>
+    <t xml:space="preserve">Ext Int Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ext Int En</t>
+  </si>
+  <si>
     <t xml:space="preserve">A7H</t>
   </si>
   <si>
@@ -5195,15 +6041,18 @@
     <t xml:space="preserve">CTC</t>
   </si>
   <si>
+    <t xml:space="preserve">min(OCR0A , OCR0B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fast PWM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved</t>
+  </si>
+  <si>
     <t xml:space="preserve">OCR0A and OCR0B</t>
   </si>
   <si>
-    <t xml:space="preserve">Fast PWM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserved</t>
-  </si>
-  <si>
     <t xml:space="preserve">WGM13</t>
   </si>
   <si>
@@ -5547,6 +6396,485 @@
   </si>
   <si>
     <t xml:space="preserve">The rising edge of INT0 generates an interrupt request.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">When </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">normal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">CTC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> mode </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[WGM02/01/00] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[WGM13/12/11/10] </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in TCCRxx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COM0A1/Β1/</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1A1/1B1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COM0A0/Β0/</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1A0/1B0</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal port operation, OC0A/Β/1A/1B disconnected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle OC0A/Β/1A/1B on compare match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear OC0A/Β/1A/1B on compare match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set OC0A/Β/1A/1B on compare match</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">When </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fast PWM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> mode </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[WGM02/01/00] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[WGM13/12/11/10] </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in TCCRxx</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM02 = 0: Normal port operation, OC0A disconnected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Reserved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM13:0 = 14 or 15: Toggle OC1A on compare match, OC1B disconnected (normal port operation). For all other WGM1 settings, normal port operation, OC1A/OC1B disconnected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM02 = 1: Toggle OC0A on compare match.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear OC0A/Β/1A/1B on match, set them at BOTTOM, (non-inverting mode)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set OC0A/Β/1A/1B on match, clear them at BOTTOM, (inverting mode).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">When </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Phase Correct PWM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Mode </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[WGM02/01/00] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[WGM13/12/11/10] </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in TCCRxx</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">WGM13:0 = 9 or 11: Toggle OC1A on compare match, OC1B disconnected (normal port operation). For all other WGM1 settings, normal port operation, OC1A/OC1B disconnected.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Clear OC0A/Β/1A/1B on compare match when </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">up-counting</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Set OC0A/Β/1A/1B on compare match when </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">down-counting</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Set OC0A/Β/1A/1B on compare match when </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">up-counting</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Clear OC0A/Β/1A/1B on compare match when </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">down-counting</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">AND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Μασκα</t>
+  </si>
+  <si>
+    <t xml:space="preserve">αποτελεσμα</t>
+  </si>
+  <si>
+    <t xml:space="preserve">αθηκτα</t>
+  </si>
+  <si>
+    <t xml:space="preserve">αντιστροφη</t>
+  </si>
+  <si>
+    <t xml:space="preserve">αθηκτο</t>
   </si>
 </sst>
 </file>
@@ -5744,22 +7072,24 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="0"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="23">
@@ -6122,7 +7452,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="88">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6363,6 +7693,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6395,11 +7729,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6407,12 +7737,72 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="9" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -6495,7 +7885,7 @@
       <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF314004"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF55308D"/>
       <rgbColor rgb="FF333333"/>
@@ -6515,7 +7905,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>384480</xdr:colOff>
+      <xdr:colOff>383040</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
@@ -6527,7 +7917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18438120" y="254160"/>
-          <a:ext cx="1859760" cy="1179000"/>
+          <a:ext cx="1858320" cy="1179000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6608,9 +7998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>140400</xdr:colOff>
+      <xdr:colOff>138960</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6620,7 +8010,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17727480" y="1233360"/>
-          <a:ext cx="338760" cy="1378080"/>
+          <a:ext cx="337320" cy="1376640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6686,7 +8076,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>436320</xdr:colOff>
+      <xdr:colOff>434880</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
@@ -6698,7 +8088,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18342360" y="1893960"/>
-          <a:ext cx="1392120" cy="336600"/>
+          <a:ext cx="1390680" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6763,9 +8153,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>139320</xdr:colOff>
+      <xdr:colOff>137880</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>145440</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6775,7 +8165,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17726400" y="2622240"/>
-          <a:ext cx="338760" cy="3481920"/>
+          <a:ext cx="337320" cy="3480480"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6841,7 +8231,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>334440</xdr:colOff>
+      <xdr:colOff>333000</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
@@ -6853,7 +8243,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18181800" y="4222800"/>
-          <a:ext cx="1450800" cy="336600"/>
+          <a:ext cx="1449360" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6918,9 +8308,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>239400</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6934,7 +8324,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="20449440" y="1835280"/>
-          <a:ext cx="4585320" cy="3027600"/>
+          <a:ext cx="4591440" cy="3026160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6955,9 +8345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>133560</xdr:colOff>
+      <xdr:colOff>132120</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6967,7 +8357,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17720640" y="517320"/>
-          <a:ext cx="338760" cy="704880"/>
+          <a:ext cx="337320" cy="703440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7034,11 +8424,11 @@
   </sheetPr>
   <dimension ref="A1:AO54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA17" activeCellId="0" sqref="AA17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R8" activeCellId="1" sqref="B3:C3 R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="8.72"/>
@@ -8128,13 +9518,13 @@
         <v>80</v>
       </c>
       <c r="X18" s="28" t="s">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="Y18" s="43" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Z18" s="33" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AA18" s="14"/>
       <c r="AB18" s="8"/>
@@ -8170,34 +9560,34 @@
         <v>84</v>
       </c>
       <c r="Q19" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="R19" s="44" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="S19" s="45" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T19" s="28" t="s">
         <v>80</v>
       </c>
       <c r="U19" s="46" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="V19" s="45" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="W19" s="46" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="X19" s="46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Y19" s="47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="Z19" s="33" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AA19" s="14"/>
       <c r="AB19" s="8"/>
@@ -8233,25 +9623,25 @@
         <v>93</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="R20" s="19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="S20" s="19" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="T20" s="48" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="U20" s="48" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="V20" s="28" t="s">
         <v>80</v>
       </c>
       <c r="W20" s="16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="X20" s="16" t="s">
         <v>51</v>
@@ -8260,7 +9650,7 @@
         <v>142</v>
       </c>
       <c r="Z20" s="33" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AA20" s="14"/>
       <c r="AB20" s="8"/>
@@ -8296,7 +9686,7 @@
         <v>101</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="R21" s="28" t="s">
         <v>80</v>
@@ -8311,19 +9701,19 @@
         <v>80</v>
       </c>
       <c r="V21" s="49" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="W21" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="X21" s="50" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Y21" s="50" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="Z21" s="33" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AA21" s="14"/>
       <c r="AB21" s="8"/>
@@ -8337,7 +9727,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -8351,10 +9741,10 @@
       <c r="K22" s="0"/>
       <c r="L22" s="0"/>
       <c r="M22" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N22" s="43" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="O22" s="43" t="s">
         <v>150</v>
@@ -8363,7 +9753,7 @@
         <v>151</v>
       </c>
       <c r="Q22" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="R22" s="51" t="s">
         <v>80</v>
@@ -8390,7 +9780,7 @@
         <v>80</v>
       </c>
       <c r="Z22" s="33" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA22" s="14"/>
       <c r="AB22" s="8"/>
@@ -8420,7 +9810,7 @@
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="R23" s="28" t="s">
         <v>80</v>
@@ -8447,7 +9837,7 @@
         <v>80</v>
       </c>
       <c r="Z23" s="33" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AA23" s="14"/>
       <c r="AB23" s="8"/>
@@ -8468,7 +9858,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="8"/>
@@ -8476,10 +9866,14 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
+      <c r="O24" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="P24" s="8" t="s">
+        <v>192</v>
+      </c>
       <c r="Q24" s="11" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="R24" s="28" t="s">
         <v>80</v>
@@ -8506,7 +9900,7 @@
         <v>80</v>
       </c>
       <c r="Z24" s="33" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AA24" s="14"/>
       <c r="AB24" s="8"/>
@@ -8533,10 +9927,14 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
+      <c r="O25" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="P25" s="35" t="s">
+        <v>105</v>
+      </c>
       <c r="Q25" s="11" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="R25" s="28" t="s">
         <v>80</v>
@@ -8563,7 +9961,7 @@
         <v>80</v>
       </c>
       <c r="Z25" s="33" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="AA25" s="14"/>
       <c r="AB25" s="8"/>
@@ -8593,25 +9991,25 @@
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="11" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="R26" s="28" t="s">
         <v>80</v>
       </c>
       <c r="S26" s="28" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="T26" s="28" t="s">
         <v>80</v>
       </c>
       <c r="U26" s="37" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="V26" s="37" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="W26" s="38" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="X26" s="16" t="s">
         <v>50</v>
@@ -8620,7 +10018,7 @@
         <v>141</v>
       </c>
       <c r="Z26" s="33" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="AA26" s="14"/>
       <c r="AB26" s="8"/>
@@ -8650,7 +10048,7 @@
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="11" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="R27" s="28" t="s">
         <v>80</v>
@@ -8659,25 +10057,25 @@
         <v>80</v>
       </c>
       <c r="T27" s="28" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="U27" s="28" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="V27" s="28" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="W27" s="28" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="X27" s="28" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="Y27" s="36" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="Z27" s="33" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AA27" s="14"/>
       <c r="AB27" s="8"/>
@@ -8707,34 +10105,34 @@
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="11" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="R28" s="28" t="s">
         <v>80</v>
       </c>
       <c r="S28" s="28" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="T28" s="28" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="U28" s="28" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="V28" s="28" t="s">
         <v>80</v>
       </c>
       <c r="W28" s="28" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="X28" s="28" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="Y28" s="36" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="Z28" s="33" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="AA28" s="14"/>
       <c r="AB28" s="8"/>
@@ -8764,7 +10162,7 @@
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
       <c r="Q29" s="11" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="R29" s="28" t="s">
         <v>80</v>
@@ -8791,7 +10189,7 @@
         <v>80</v>
       </c>
       <c r="Z29" s="33" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="AA29" s="14"/>
       <c r="AB29" s="8"/>
@@ -8805,7 +10203,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -8823,7 +10221,7 @@
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="11" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="R30" s="28" t="s">
         <v>80</v>
@@ -8850,7 +10248,7 @@
         <v>80</v>
       </c>
       <c r="Z30" s="33" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="AA30" s="14"/>
       <c r="AB30" s="8"/>
@@ -8880,7 +10278,7 @@
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
       <c r="Q31" s="11" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="R31" s="28" t="s">
         <v>80</v>
@@ -8907,7 +10305,7 @@
         <v>80</v>
       </c>
       <c r="Z31" s="33" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="AA31" s="14"/>
       <c r="AB31" s="8"/>
@@ -8937,7 +10335,7 @@
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
       <c r="Q32" s="11" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="R32" s="28" t="s">
         <v>80</v>
@@ -8964,7 +10362,7 @@
         <v>80</v>
       </c>
       <c r="Z32" s="33" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="AA32" s="14"/>
       <c r="AB32" s="8"/>
@@ -8994,7 +10392,7 @@
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
       <c r="Q33" s="11" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="R33" s="28" t="s">
         <v>80</v>
@@ -9021,7 +10419,7 @@
         <v>80</v>
       </c>
       <c r="Z33" s="33" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="AA33" s="14"/>
       <c r="AB33" s="8"/>
@@ -9051,7 +10449,7 @@
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
       <c r="Q34" s="11" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="R34" s="28" t="s">
         <v>80</v>
@@ -9078,7 +10476,7 @@
         <v>80</v>
       </c>
       <c r="Z34" s="33" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="AA34" s="14"/>
       <c r="AB34" s="8"/>
@@ -9108,7 +10506,7 @@
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
       <c r="Q35" s="11" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="R35" s="28" t="s">
         <v>80</v>
@@ -9132,10 +10530,10 @@
         <v>139</v>
       </c>
       <c r="Y35" s="53" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="Z35" s="33" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AA35" s="14"/>
       <c r="AB35" s="8"/>
@@ -9273,8 +10671,8 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="B3:C3 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9309,37 +10707,40 @@
       <c r="D2" s="39" t="s">
         <v>141</v>
       </c>
+      <c r="F2" s="56" t="s">
+        <v>159</v>
+      </c>
       <c r="G2" s="57" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="58" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="H3" s="59" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9356,16 +10757,16 @@
         <v>0</v>
       </c>
       <c r="E4" s="56" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G4" s="56" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="H4" s="56" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9382,16 +10783,16 @@
         <v>1</v>
       </c>
       <c r="E5" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="F5" s="56" t="s">
         <v>246</v>
       </c>
-      <c r="F5" s="56" t="s">
-        <v>243</v>
-      </c>
       <c r="G5" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H5" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9408,16 +10809,16 @@
         <v>0</v>
       </c>
       <c r="E6" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>252</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="H6" s="56" t="s">
         <v>248</v>
-      </c>
-      <c r="F6" s="60" t="s">
-        <v>249</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>244</v>
-      </c>
-      <c r="H6" s="56" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9434,16 +10835,16 @@
         <v>1</v>
       </c>
       <c r="E7" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="F7" s="56" t="s">
-        <v>243</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>247</v>
-      </c>
       <c r="H7" s="56" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9460,7 +10861,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F8" s="56" t="s">
         <v>80</v>
@@ -9486,16 +10887,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="F9" s="60" t="s">
         <v>249</v>
       </c>
+      <c r="F9" s="61" t="s">
+        <v>255</v>
+      </c>
       <c r="G9" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H9" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9512,7 +10913,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F10" s="56" t="s">
         <v>80</v>
@@ -9538,16 +10939,16 @@
         <v>1</v>
       </c>
       <c r="E11" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>255</v>
+      </c>
+      <c r="G11" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="F11" s="60" t="s">
-        <v>249</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>247</v>
-      </c>
       <c r="H11" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9564,39 +10965,39 @@
         <v>142</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="I14" s="57" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="58" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F15" s="58" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G15" s="58" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H15" s="59" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="I15" s="59" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9616,16 +11017,16 @@
         <v>0</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G16" s="56" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="H16" s="56" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9645,16 +11046,16 @@
         <v>1</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="G17" s="56" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="H17" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I17" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9674,16 +11075,16 @@
         <v>0</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="G18" s="56" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="H18" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I18" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9703,16 +11104,16 @@
         <v>1</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="G19" s="56" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="H19" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I19" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9732,16 +11133,16 @@
         <v>0</v>
       </c>
       <c r="F20" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="G20" s="56" t="s">
+        <v>267</v>
+      </c>
+      <c r="H20" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I20" s="56" t="s">
         <v>248</v>
-      </c>
-      <c r="G20" s="56" t="s">
-        <v>263</v>
-      </c>
-      <c r="H20" s="56" t="s">
-        <v>244</v>
-      </c>
-      <c r="I20" s="56" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9761,16 +11162,16 @@
         <v>1</v>
       </c>
       <c r="F21" s="56" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="G21" s="56" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="H21" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I21" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9790,16 +11191,16 @@
         <v>0</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="G22" s="56" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="H22" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I22" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9819,16 +11220,16 @@
         <v>1</v>
       </c>
       <c r="F23" s="56" t="s">
+        <v>270</v>
+      </c>
+      <c r="G23" s="56" t="s">
         <v>266</v>
       </c>
-      <c r="G23" s="56" t="s">
-        <v>262</v>
-      </c>
       <c r="H23" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I23" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9848,16 +11249,16 @@
         <v>0</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="G24" s="56" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H24" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I24" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9877,16 +11278,16 @@
         <v>1</v>
       </c>
       <c r="F25" s="56" t="s">
+        <v>271</v>
+      </c>
+      <c r="G25" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="G25" s="56" t="s">
-        <v>263</v>
-      </c>
       <c r="H25" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I25" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9906,16 +11307,16 @@
         <v>0</v>
       </c>
       <c r="F26" s="56" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G26" s="56" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H26" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I26" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9935,16 +11336,16 @@
         <v>1</v>
       </c>
       <c r="F27" s="56" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G27" s="56" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H27" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I27" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9964,16 +11365,16 @@
         <v>0</v>
       </c>
       <c r="F28" s="56" t="s">
+        <v>251</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="H28" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="I28" s="56" t="s">
         <v>248</v>
-      </c>
-      <c r="G28" s="56" t="s">
-        <v>268</v>
-      </c>
-      <c r="H28" s="56" t="s">
-        <v>244</v>
-      </c>
-      <c r="I28" s="56" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9993,7 +11394,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="56" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="G29" s="56" t="s">
         <v>80</v>
@@ -10022,16 +11423,16 @@
         <v>0</v>
       </c>
       <c r="F30" s="56" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="G30" s="56" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H30" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I30" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10051,16 +11452,16 @@
         <v>1</v>
       </c>
       <c r="F31" s="56" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="G31" s="56" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="H31" s="56" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="I31" s="56" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -10082,11 +11483,11 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="B3:C3 A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
@@ -10094,7 +11495,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>52</v>
@@ -10123,20 +11524,20 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="56" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>274</v>
-      </c>
-      <c r="D2" s="61" t="s">
-        <v>275</v>
-      </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
+        <v>278</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>279</v>
+      </c>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
       <c r="H2" s="56"/>
       <c r="I2" s="56"/>
       <c r="J2" s="56"/>
@@ -10154,13 +11555,13 @@
       <c r="C3" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="62" t="s">
-        <v>276</v>
-      </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
+      <c r="D3" s="63" t="s">
+        <v>280</v>
+      </c>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
       <c r="I3" s="56"/>
       <c r="J3" s="56"/>
       <c r="K3" s="56"/>
@@ -10177,13 +11578,13 @@
       <c r="C4" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="62" t="s">
-        <v>277</v>
-      </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="D4" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
       <c r="I4" s="56"/>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
@@ -10200,13 +11601,13 @@
       <c r="C5" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="62" t="s">
-        <v>278</v>
-      </c>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="D5" s="63" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
       <c r="I5" s="56"/>
       <c r="J5" s="56"/>
       <c r="K5" s="56"/>
@@ -10223,13 +11624,13 @@
       <c r="C6" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="62" t="s">
-        <v>279</v>
-      </c>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
+      <c r="D6" s="63" t="s">
+        <v>283</v>
+      </c>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="56"/>
       <c r="J6" s="56"/>
       <c r="K6" s="56"/>
@@ -10246,13 +11647,13 @@
       <c r="C7" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="62" t="s">
-        <v>280</v>
-      </c>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
+      <c r="D7" s="63" t="s">
+        <v>284</v>
+      </c>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
       <c r="I7" s="56"/>
       <c r="J7" s="56"/>
       <c r="K7" s="56"/>
@@ -10269,13 +11670,13 @@
       <c r="C8" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="62" t="s">
-        <v>281</v>
-      </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
+      <c r="D8" s="63" t="s">
+        <v>285</v>
+      </c>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
       <c r="I8" s="56"/>
       <c r="J8" s="56"/>
       <c r="K8" s="56"/>
@@ -10292,18 +11693,18 @@
       <c r="C9" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="62" t="s">
-        <v>282</v>
-      </c>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
+      <c r="D9" s="63" t="s">
+        <v>286</v>
+      </c>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="56" t="n">
@@ -10315,18 +11716,18 @@
       <c r="C10" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="62" t="s">
-        <v>283</v>
-      </c>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
+      <c r="D10" s="63" t="s">
+        <v>287</v>
+      </c>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
@@ -10341,20 +11742,20 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="56" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>286</v>
-      </c>
-      <c r="D13" s="61" t="s">
-        <v>287</v>
-      </c>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
+        <v>290</v>
+      </c>
+      <c r="D13" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
       <c r="H13" s="56"/>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
@@ -10372,18 +11773,18 @@
       <c r="C14" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="62" t="s">
-        <v>288</v>
-      </c>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
+      <c r="D14" s="63" t="s">
+        <v>292</v>
+      </c>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="56" t="n">
@@ -10395,18 +11796,18 @@
       <c r="C15" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="62" t="s">
-        <v>289</v>
-      </c>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="M15" s="63"/>
+      <c r="D15" s="63" t="s">
+        <v>293</v>
+      </c>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="56" t="n">
@@ -10418,18 +11819,18 @@
       <c r="C16" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="62" t="s">
-        <v>290</v>
-      </c>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
-      <c r="M16" s="63"/>
+      <c r="D16" s="63" t="s">
+        <v>294</v>
+      </c>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="56" t="n">
@@ -10441,18 +11842,18 @@
       <c r="C17" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="62" t="s">
-        <v>291</v>
-      </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="63"/>
-      <c r="L17" s="63"/>
-      <c r="M17" s="63"/>
+      <c r="D17" s="63" t="s">
+        <v>295</v>
+      </c>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="56" t="n">
@@ -10464,18 +11865,18 @@
       <c r="C18" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D18" s="62" t="s">
-        <v>292</v>
-      </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
-      <c r="L18" s="63"/>
-      <c r="M18" s="63"/>
+      <c r="D18" s="63" t="s">
+        <v>296</v>
+      </c>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="56" t="n">
@@ -10487,18 +11888,18 @@
       <c r="C19" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="62" t="s">
-        <v>293</v>
-      </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="63"/>
-      <c r="L19" s="63"/>
-      <c r="M19" s="63"/>
+      <c r="D19" s="63" t="s">
+        <v>297</v>
+      </c>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="56" t="n">
@@ -10510,18 +11911,18 @@
       <c r="C20" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="62" t="s">
-        <v>294</v>
-      </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="63"/>
-      <c r="L20" s="63"/>
-      <c r="M20" s="63"/>
+      <c r="D20" s="63" t="s">
+        <v>298</v>
+      </c>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="56" t="n">
@@ -10533,27 +11934,27 @@
       <c r="C21" s="56" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="62" t="s">
-        <v>295</v>
-      </c>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
+      <c r="D21" s="63" t="s">
+        <v>299</v>
+      </c>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="64" t="s">
-        <v>296</v>
-      </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
+      <c r="A23" s="65" t="s">
+        <v>300</v>
+      </c>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10604,310 +12005,310 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
-        <v>297</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>298</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>299</v>
+      <c r="A1" s="66" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="67" t="n">
+      <c r="A2" s="68" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="68" t="s">
-        <v>300</v>
-      </c>
-      <c r="C2" s="68" t="s">
-        <v>301</v>
+      <c r="B2" s="60" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="67" t="n">
+      <c r="A3" s="68" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="68" t="s">
-        <v>302</v>
-      </c>
-      <c r="C3" s="68" t="s">
-        <v>303</v>
+      <c r="B3" s="60" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="67" t="n">
+      <c r="A4" s="68" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="68" t="s">
-        <v>304</v>
-      </c>
-      <c r="C4" s="68" t="s">
-        <v>305</v>
+      <c r="B4" s="60" t="s">
+        <v>308</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="67" t="n">
+      <c r="A5" s="68" t="n">
         <v>6</v>
       </c>
-      <c r="B5" s="68" t="s">
-        <v>306</v>
-      </c>
-      <c r="C5" s="68" t="s">
-        <v>307</v>
+      <c r="B5" s="60" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="67" t="n">
+      <c r="A6" s="68" t="n">
         <v>8</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>308</v>
-      </c>
-      <c r="C6" s="68" t="s">
-        <v>307</v>
+      <c r="B6" s="60" t="s">
+        <v>312</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="68" t="s">
-        <v>309</v>
-      </c>
-      <c r="B7" s="68" t="s">
-        <v>310</v>
-      </c>
-      <c r="C7" s="68" t="s">
-        <v>311</v>
+      <c r="A7" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="68" t="s">
-        <v>312</v>
-      </c>
-      <c r="B8" s="68" t="s">
-        <v>313</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>314</v>
+      <c r="A8" s="60" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="68" t="s">
-        <v>315</v>
-      </c>
-      <c r="B9" s="68" t="s">
+      <c r="A9" s="60" t="s">
+        <v>319</v>
+      </c>
+      <c r="B9" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="68" t="s">
-        <v>316</v>
+      <c r="C9" s="60" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="67" t="n">
+      <c r="A10" s="68" t="n">
         <v>10</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="68" t="s">
-        <v>316</v>
+      <c r="C10" s="60" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="67" t="n">
+      <c r="A11" s="68" t="n">
         <v>12</v>
       </c>
-      <c r="B11" s="68" t="s">
-        <v>317</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>318</v>
+      <c r="B11" s="60" t="s">
+        <v>321</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="67" t="n">
+      <c r="A12" s="68" t="n">
         <v>14</v>
       </c>
-      <c r="B12" s="68" t="s">
-        <v>319</v>
-      </c>
-      <c r="C12" s="68" t="s">
-        <v>320</v>
+      <c r="B12" s="60" t="s">
+        <v>323</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="67" t="n">
+      <c r="A13" s="68" t="n">
         <v>16</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="68" t="s">
-        <v>321</v>
+      <c r="C13" s="60" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="67" t="n">
+      <c r="A14" s="68" t="n">
         <v>18</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="68" t="s">
-        <v>322</v>
+      <c r="C14" s="60" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="68" t="s">
-        <v>323</v>
-      </c>
-      <c r="B15" s="68" t="s">
-        <v>324</v>
-      </c>
-      <c r="C15" s="68" t="s">
-        <v>325</v>
+      <c r="A15" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="68" t="s">
-        <v>326</v>
-      </c>
-      <c r="B16" s="68" t="s">
+      <c r="A16" s="60" t="s">
+        <v>330</v>
+      </c>
+      <c r="B16" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="68" t="s">
-        <v>327</v>
+      <c r="C16" s="60" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="68" t="s">
-        <v>328</v>
-      </c>
-      <c r="B17" s="68" t="s">
+      <c r="A17" s="60" t="s">
+        <v>332</v>
+      </c>
+      <c r="B17" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="68" t="s">
-        <v>329</v>
+      <c r="C17" s="60" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="67" t="n">
+      <c r="A18" s="68" t="n">
         <v>20</v>
       </c>
-      <c r="B18" s="68" t="s">
-        <v>330</v>
-      </c>
-      <c r="C18" s="68" t="s">
-        <v>331</v>
+      <c r="B18" s="60" t="s">
+        <v>334</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="67" t="n">
+      <c r="A19" s="68" t="n">
         <v>22</v>
       </c>
-      <c r="B19" s="68" t="s">
-        <v>332</v>
-      </c>
-      <c r="C19" s="68" t="s">
-        <v>333</v>
+      <c r="B19" s="60" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="67" t="n">
+      <c r="A20" s="68" t="n">
         <v>24</v>
       </c>
-      <c r="B20" s="68" t="s">
-        <v>334</v>
-      </c>
-      <c r="C20" s="68" t="s">
-        <v>335</v>
+      <c r="B20" s="60" t="s">
+        <v>338</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="67" t="n">
+      <c r="A21" s="68" t="n">
         <v>26</v>
       </c>
-      <c r="B21" s="68" t="s">
-        <v>336</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>337</v>
+      <c r="B21" s="60" t="s">
+        <v>340</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="67" t="n">
+      <c r="A22" s="68" t="n">
         <v>28</v>
       </c>
-      <c r="B22" s="68" t="s">
-        <v>338</v>
-      </c>
-      <c r="C22" s="68" t="s">
-        <v>339</v>
+      <c r="B22" s="60" t="s">
+        <v>342</v>
+      </c>
+      <c r="C22" s="60" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="68" t="s">
-        <v>340</v>
-      </c>
-      <c r="B23" s="68" t="s">
-        <v>341</v>
-      </c>
-      <c r="C23" s="68" t="s">
-        <v>342</v>
+      <c r="A23" s="60" t="s">
+        <v>344</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>345</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="68" t="s">
-        <v>343</v>
-      </c>
-      <c r="B24" s="68" t="s">
-        <v>344</v>
-      </c>
-      <c r="C24" s="68" t="s">
-        <v>345</v>
+      <c r="A24" s="60" t="s">
+        <v>347</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>348</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="68" t="s">
-        <v>346</v>
-      </c>
-      <c r="B25" s="68" t="s">
-        <v>347</v>
-      </c>
-      <c r="C25" s="68" t="s">
-        <v>348</v>
+      <c r="A25" s="60" t="s">
+        <v>350</v>
+      </c>
+      <c r="B25" s="60" t="s">
+        <v>351</v>
+      </c>
+      <c r="C25" s="60" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="67" t="n">
+      <c r="A26" s="68" t="n">
         <v>30</v>
       </c>
-      <c r="B26" s="68" t="s">
-        <v>349</v>
-      </c>
-      <c r="C26" s="68" t="s">
-        <v>350</v>
+      <c r="B26" s="60" t="s">
+        <v>353</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="67" t="n">
+      <c r="A27" s="68" t="n">
         <v>32</v>
       </c>
-      <c r="B27" s="68" t="s">
-        <v>351</v>
-      </c>
-      <c r="C27" s="68" t="s">
-        <v>352</v>
+      <c r="B27" s="60" t="s">
+        <v>355</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -10928,13 +12329,13 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="56" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="56" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10950,18 +12351,18 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="70" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>354</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>355</v>
-      </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+        <v>358</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="70" t="n">
@@ -10970,17 +12371,17 @@
       <c r="B4" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="71" t="s">
-        <v>356</v>
-      </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
+      <c r="C4" s="63" t="s">
+        <v>360</v>
+      </c>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="70" t="n">
@@ -10989,17 +12390,17 @@
       <c r="B5" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="71" t="s">
-        <v>357</v>
-      </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="C5" s="63" t="s">
+        <v>361</v>
+      </c>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="70" t="n">
@@ -11008,17 +12409,17 @@
       <c r="B6" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="71" t="s">
-        <v>358</v>
-      </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
+      <c r="C6" s="63" t="s">
+        <v>362</v>
+      </c>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="70" t="n">
@@ -11027,17 +12428,17 @@
       <c r="B7" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="71" t="s">
-        <v>359</v>
-      </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
+      <c r="C7" s="63" t="s">
+        <v>363</v>
+      </c>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="70"/>
@@ -11049,18 +12450,18 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="70" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>361</v>
-      </c>
-      <c r="C11" s="72" t="s">
-        <v>362</v>
-      </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
+        <v>365</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>366</v>
+      </c>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="70" t="n">
@@ -11069,17 +12470,17 @@
       <c r="B12" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="71" t="s">
-        <v>363</v>
-      </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
+      <c r="C12" s="63" t="s">
+        <v>367</v>
+      </c>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="70" t="n">
@@ -11088,17 +12489,17 @@
       <c r="B13" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="71" t="s">
-        <v>364</v>
-      </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="63"/>
+      <c r="C13" s="63" t="s">
+        <v>368</v>
+      </c>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="70" t="n">
@@ -11107,17 +12508,17 @@
       <c r="B14" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="71" t="s">
-        <v>365</v>
-      </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
+      <c r="C14" s="63" t="s">
+        <v>369</v>
+      </c>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="70" t="n">
@@ -11126,17 +12527,17 @@
       <c r="B15" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="71" t="s">
-        <v>366</v>
-      </c>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
+      <c r="C15" s="63" t="s">
+        <v>370</v>
+      </c>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -11160,4 +12561,485 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="B3:C3 A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="56" width="20.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="56" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="56" width="31.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="56" width="10"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="56" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="69" t="s">
+        <v>371</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="70" t="s">
+        <v>372</v>
+      </c>
+      <c r="B2" s="70" t="s">
+        <v>373</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>375</v>
+      </c>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="64"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>376</v>
+      </c>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="64"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>378</v>
+      </c>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="64"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="69" t="s">
+        <v>379</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="70" t="s">
+        <v>372</v>
+      </c>
+      <c r="B9" s="70" t="s">
+        <v>373</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="73" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>375</v>
+      </c>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+    </row>
+    <row r="11" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>380</v>
+      </c>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="76" t="s">
+        <v>381</v>
+      </c>
+      <c r="H11" s="77" t="s">
+        <v>382</v>
+      </c>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="77"/>
+    </row>
+    <row r="12" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="63" t="s">
+        <v>383</v>
+      </c>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>384</v>
+      </c>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>385</v>
+      </c>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="69" t="s">
+        <v>386</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="70" t="s">
+        <v>372</v>
+      </c>
+      <c r="B17" s="70" t="s">
+        <v>373</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>374</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="73" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="78" t="s">
+        <v>375</v>
+      </c>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+    </row>
+    <row r="19" customFormat="false" ht="22.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="B19" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="80" t="s">
+        <v>380</v>
+      </c>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="76" t="s">
+        <v>381</v>
+      </c>
+      <c r="H19" s="81" t="s">
+        <v>387</v>
+      </c>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+    </row>
+    <row r="20" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="79"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="82" t="s">
+        <v>383</v>
+      </c>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="80" t="s">
+        <v>388</v>
+      </c>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="79"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="83" t="s">
+        <v>389</v>
+      </c>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="84" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="84" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="80" t="s">
+        <v>390</v>
+      </c>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="84"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="82" t="s">
+        <v>391</v>
+      </c>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:K12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:K20"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="85"/>
+      <c r="B1" s="70" t="s">
+        <v>392</v>
+      </c>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70" t="s">
+        <v>394</v>
+      </c>
+      <c r="G1" s="70"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="86" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" s="86" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="86" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="86" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="87" t="s">
+        <v>396</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>397</v>
+      </c>
+      <c r="C3" s="87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="87" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="87" t="s">
+        <v>397</v>
+      </c>
+      <c r="F3" s="87" t="s">
+        <v>398</v>
+      </c>
+      <c r="G3" s="87" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
main functions done. debugging remaining
</commit_message>
<xml_diff>
--- a/[1]Atmega328p map & datasheet/Atmega328p.xlsx
+++ b/[1]Atmega328p map & datasheet/Atmega328p.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" state="visible" r:id="rId2"/>
@@ -673,6 +673,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">[PD3]
+	ISR(INT1_vect){}
 </t>
         </r>
         <r>
@@ -717,7 +718,18 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">[PD2]</t>
+          <t xml:space="preserve">[PD2]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">	ISR(INT0_vect){}</t>
         </r>
       </text>
     </comment>
@@ -6853,13 +6865,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">AND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XOR</t>
+    <t xml:space="preserve">AND ( &amp; )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR ( | )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XOR ( ^ )</t>
   </si>
   <si>
     <t xml:space="preserve">Μασκα</t>
@@ -6885,7 +6897,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -7070,6 +7082,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -7745,7 +7764,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="9" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="9" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7797,7 +7816,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7905,7 +7924,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>383040</xdr:colOff>
+      <xdr:colOff>382320</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
@@ -7917,7 +7936,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18438120" y="254160"/>
-          <a:ext cx="1858320" cy="1179000"/>
+          <a:ext cx="1857600" cy="1179000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7998,9 +8017,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>138960</xdr:colOff>
+      <xdr:colOff>138240</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8010,7 +8029,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17727480" y="1233360"/>
-          <a:ext cx="337320" cy="1376640"/>
+          <a:ext cx="336600" cy="1375920"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8076,7 +8095,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>434880</xdr:colOff>
+      <xdr:colOff>434160</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
@@ -8088,7 +8107,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18342360" y="1893960"/>
-          <a:ext cx="1390680" cy="336600"/>
+          <a:ext cx="1389960" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8153,9 +8172,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>137880</xdr:colOff>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8165,7 +8184,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17726400" y="2622240"/>
-          <a:ext cx="337320" cy="3480480"/>
+          <a:ext cx="336600" cy="3479760"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8231,7 +8250,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
@@ -8243,7 +8262,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18181800" y="4222800"/>
-          <a:ext cx="1449360" cy="336600"/>
+          <a:ext cx="1448640" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8308,9 +8327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>239400</xdr:colOff>
+      <xdr:colOff>238680</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8324,7 +8343,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="20449440" y="1835280"/>
-          <a:ext cx="4591440" cy="3026160"/>
+          <a:ext cx="4594680" cy="3025440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8345,9 +8364,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>132120</xdr:colOff>
+      <xdr:colOff>131400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8357,7 +8376,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17720640" y="517320"/>
-          <a:ext cx="337320" cy="703440"/>
+          <a:ext cx="336600" cy="702720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8424,11 +8443,11 @@
   </sheetPr>
   <dimension ref="A1:AO54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R8" activeCellId="1" sqref="B3:C3 R8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V18" activeCellId="0" sqref="V18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="8.72"/>
@@ -10672,7 +10691,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="B3:C3 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11484,10 +11503,10 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="B3:C3 A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
@@ -12006,10 +12025,10 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="B3:C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.32"/>
   </cols>
@@ -12330,10 +12349,10 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="B3:C3"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="56" width="11.52"/>
   </cols>
@@ -12571,7 +12590,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="B3:C3 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12960,26 +12979,26 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="85"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="71" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70" t="s">
+      <c r="C1" s="71"/>
+      <c r="D1" s="71" t="s">
         <v>393</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70" t="s">
+      <c r="E1" s="71"/>
+      <c r="F1" s="71" t="s">
         <v>394</v>
       </c>
-      <c r="G1" s="70"/>
+      <c r="G1" s="71"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="86" t="s">

</xml_diff>